<commit_message>
Added hand drawn cube map (based on measured environment map of balls 1 & 4)
</commit_message>
<xml_diff>
--- a/Documentation/Original.xlsx
+++ b/Documentation/Original.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="374">
   <si>
     <t>Pixelwidth</t>
   </si>
@@ -1071,6 +1071,81 @@
   </si>
   <si>
     <t>194,8 mm</t>
+  </si>
+  <si>
+    <t>Number on Ball 9a</t>
+  </si>
+  <si>
+    <t>Number on Ball 9b</t>
+  </si>
+  <si>
+    <t>Number on Ball 9c</t>
+  </si>
+  <si>
+    <t>78,7338 mm</t>
+  </si>
+  <si>
+    <t>181,5186 mm</t>
+  </si>
+  <si>
+    <t>24 mm</t>
+  </si>
+  <si>
+    <t>15,2398 mm</t>
+  </si>
+  <si>
+    <t>41 deg</t>
+  </si>
+  <si>
+    <t>82,25 mm</t>
+  </si>
+  <si>
+    <t>178,5 mm</t>
+  </si>
+  <si>
+    <t>77,05 mm</t>
+  </si>
+  <si>
+    <t>186,8 mm</t>
+  </si>
+  <si>
+    <t>88,1052 mm</t>
+  </si>
+  <si>
+    <t>167,0008 mm</t>
+  </si>
+  <si>
+    <t>30 deg</t>
+  </si>
+  <si>
+    <t>92,375 mm</t>
+  </si>
+  <si>
+    <t>168,125 mm</t>
+  </si>
+  <si>
+    <t>87 mm</t>
+  </si>
+  <si>
+    <t>177,5 mm</t>
+  </si>
+  <si>
+    <t>90,1225 mm</t>
+  </si>
+  <si>
+    <t>162,9565 mm</t>
+  </si>
+  <si>
+    <t>88,25 mm</t>
+  </si>
+  <si>
+    <t>157 mm</t>
+  </si>
+  <si>
+    <t>90,725 mm</t>
+  </si>
+  <si>
+    <t>167,375 mm</t>
   </si>
 </sst>
 </file>
@@ -1133,10 +1208,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1419,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U199"/>
+  <dimension ref="A1:U212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="G182" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L214" sqref="L214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,12 +1546,12 @@
       <c r="H2" t="s">
         <v>309</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="5" t="str">
         <f>"new ColorRef { PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F2,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
@@ -1509,12 +1584,12 @@
       <c r="H3" t="s">
         <v>310</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
       <c r="M3" s="5" t="str">
         <f t="shared" ref="M3:M12" si="0">"new ColorRef { PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F3,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
@@ -1545,12 +1620,12 @@
       <c r="H4" t="s">
         <v>313</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
       <c r="M4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(86.20f, 287.82f), Radius = 35.91f }, // Cloth with shadow of lamp 1 (highest)</v>
@@ -1578,12 +1653,12 @@
       <c r="H5" t="s">
         <v>316</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
       <c r="M5" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(398.50f, 575.20f), Radius = 20.52f }, // Cloth with shadow of lamp 2</v>
@@ -1611,12 +1686,12 @@
       <c r="H6" t="s">
         <v>319</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
       <c r="M6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(444.56f, 449.02f), Radius = 30.99f }, // Cloth with shadow of lamp 3 (lowest)</v>
@@ -1644,12 +1719,12 @@
       <c r="H7" t="s">
         <v>322</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(83.24f, 134.94f), Radius = 20.41f }, // Lightest part of Ball 1</v>
@@ -1668,12 +1743,12 @@
       <c r="H8" t="s">
         <v>322</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
       <c r="M8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(709.32f, 99.04f), Radius = 20.41f }, // Lightest part of Ball 4</v>
@@ -1683,7 +1758,7 @@
       <c r="A9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="8" t="str">
+      <c r="B9" s="7" t="str">
         <f>"new Ball { Name = """ &amp; A9 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B10,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B11,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -1692,8 +1767,8 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B14,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 1", PixelCenter = new PointF(111.78f, 166.22f), PixelSize = new SizeF(175.02f, 176.32f), Degrees = -179.50f },</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9">
         <v>7</v>
       </c>
@@ -1736,12 +1811,12 @@
       <c r="H10" t="s">
         <v>339</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(621.44f, 73.33f), Radius = 18.90f }, // Reflection of cloth in Ball 4</v>
@@ -1766,12 +1841,12 @@
       <c r="H11" t="s">
         <v>343</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(111.02f, 169.15f), Radius = 12.47f }, // White part of the number texture</v>
@@ -1824,7 +1899,7 @@
       <c r="A16" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B16" s="8" t="str">
+      <c r="B16" s="7" t="str">
         <f>"new Ball { Name = """ &amp; A16 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -1833,12 +1908,12 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 9a", PixelCenter = new PointF(326.64f, 247.57f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F16" s="8" t="str">
+      <c r="F16" s="7" t="str">
         <f>"new Ball { Name = """ &amp; E16 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(F18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -1847,12 +1922,12 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(F21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 9b", PixelCenter = new PointF(337.32f, 267.88f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J16" s="8" t="str">
+      <c r="J16" s="7" t="str">
         <f>"new Ball { Name = """ &amp; I16 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(J17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(J18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -1861,8 +1936,8 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(J21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 9c", PixelCenter = new PointF(340.62f, 297.17f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
       <c r="Q16" s="2"/>
       <c r="U16" s="2"/>
     </row>
@@ -1970,7 +2045,7 @@
       <c r="A23" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B23" s="8" t="str">
+      <c r="B23" s="7" t="str">
         <f>"new Ball { Name = """ &amp; A23 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B24,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B25,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -1979,12 +2054,12 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 8a", PixelCenter = new PointF(513.15f, 187.86f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F23" s="8" t="str">
+      <c r="F23" s="7" t="str">
         <f>"new Ball { Name = """ &amp; E23 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F24,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(F25,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -1993,8 +2068,8 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(F28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 8b", PixelCenter = new PointF(495.39f, 193.06f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -2072,7 +2147,7 @@
       <c r="A30" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B30" s="8" t="str">
+      <c r="B30" s="7" t="str">
         <f>"new Ball { Name = """ &amp; A30 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B31,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B32,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -2081,8 +2156,8 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B35,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 4", PixelCenter = new PointF(675.32f, 122.76f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2130,7 +2205,7 @@
       <c r="A37" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B37" s="8" t="str">
+      <c r="B37" s="7" t="str">
         <f>"new Ball { Name = """ &amp; A37 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B38,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B39,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -2139,8 +2214,8 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B42,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball w", PixelCenter = new PointF(296.49f, 550.67f), PixelSize = new SizeF(177.64f, 177.64f), Degrees = -19.00f },</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2202,21 +2277,21 @@
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="8" t="str">
+      <c r="B46" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C51, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C52, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C53, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C54, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C55, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C56, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C57, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C58, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (133.742761814912f, 205.892540265516f), new PointF(137.83334515448f, 202.417265656646f), new PointF(140.168715611395f, 205.047438142032f), new PointF(136.177533862726f, 208.63383082975f) },</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
       <c r="F46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G46" s="8" t="str">
+      <c r="G46" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H51, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H52, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H53, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H54, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H55, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H56, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H57, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H58, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (699.875451915949f, 164.6093393286f), new PointF(703.879106107581f, 161.802662956064f), new PointF(705.755263891709f, 165.080646282082f), new PointF(700.908774917924f, 168.021873797712f) },</v>
       </c>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
       <c r="K46" s="2"/>
       <c r="M46"/>
       <c r="Q46" s="2"/>
@@ -2533,21 +2608,21 @@
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="8" t="str">
+      <c r="B60" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C65, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C66, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C67, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C68, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C69, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C70, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C71, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C72, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (138.596053939405f, 201.709927273775f), new PointF(149.288339135411f, 188.969143471165f), new PointF(152.571237304817f, 191.438686080665f), new PointF(140.923865339978f, 204.331028895582f) },</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
       <c r="F60" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G60" s="8" t="str">
+      <c r="G60" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H65, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H66, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H67, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H68, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H69, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H70, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H71, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H72, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (704.847421225014f, 161.05715135563f), new PointF(717.414352393879f, 148.062005420146f), new PointF(720.371077282121f, 151.265154121633f), new PointF(706.79312232749f, 164.366882704175f) },</v>
       </c>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
       <c r="K60" s="2"/>
       <c r="M60"/>
       <c r="Q60" s="2"/>
@@ -2864,21 +2939,21 @@
       <c r="A74" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B74" s="8" t="str">
+      <c r="B74" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C79, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C80, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C81, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C82, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C83, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C84, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C85, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C86, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (149.881725058272f, 188.044293338712f), new PointF(152.033788398889f, 184.38004240527f), new PointF(156.288025308265f, 186.401333172887f), new PointF(153.240969696734f, 190.571284750882f) },</v>
       </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
       <c r="F74" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G74" s="8" t="str">
+      <c r="G74" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H79, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H80, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H81, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H82, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H83, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H84, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H85, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H86, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (718.239423393628f, 146.901312834628f), new PointF(721.061219126161f, 142.460369207198f), new PointF(724.375487379388f, 145.268935342979f), new PointF(721.251707345984f, 150.072335560938f) },</v>
       </c>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
       <c r="K74" s="2"/>
       <c r="M74"/>
       <c r="Q74" s="2"/>
@@ -3195,21 +3270,21 @@
       <c r="A88" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B88" s="8" t="str">
+      <c r="B88" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C93, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C94, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C95, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C96, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C97, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C98, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C99, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C100, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (136.019738561583f, 209.782050977847f), new PointF(157.075490002711f, 186.775695271863f), new PointF(162.124561686466f, 189.174182783325f), new PointF(141.012117322773f, 215.415435213323f) },</v>
       </c>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
       <c r="F88" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G88" s="8" t="str">
+      <c r="G88" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H93, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H94, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H95, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H96, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H97, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H98, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H99, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H100, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (701.232680482186f, 169.09242467641f), new PointF(725.421282824328f, 146.15523430522f), new PointF(730.386826935502f, 150.363737053427f), new PointF(703.400617841122f, 176.252359661775f) },</v>
       </c>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
       <c r="K88" s="2"/>
       <c r="M88"/>
       <c r="Q88" s="2"/>
@@ -3526,21 +3601,21 @@
       <c r="A102" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B102" s="8" t="str">
+      <c r="B102" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C107, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C108, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C109, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C110, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C111, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C112, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C113, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C114, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (152.642670387251f, 183.239003357508f), new PointF(160.004813311712f, 159.493372269801f), new PointF(161.714293903495f, 159.475608495291f), new PointF(154.205883238813f, 183.981680313074f) },</v>
       </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
       <c r="F102" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G102" s="8" t="str">
+      <c r="G102" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H107, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H108, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H109, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H110, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H111, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H112, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H113, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H114, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (721.855486971315f, 141.048527086324f), new PointF(729.501472461425f, 116.638455241424f), new PointF(731.432811356851f, 116.698171759988f), new PointF(723.65227466385f, 142.57167626237f) },</v>
       </c>
-      <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
+      <c r="H102" s="7"/>
+      <c r="I102" s="7"/>
       <c r="K102" s="2"/>
       <c r="M102"/>
       <c r="Q102" s="2"/>
@@ -3857,21 +3932,21 @@
       <c r="A116" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B116" s="8" t="str">
+      <c r="B116" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C121, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C122, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C123, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C124, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C125, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C126, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C127, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C128, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (155.202544817528f, 184.45525498245f), new PointF(162.703774378685f, 159.465403773764f), new PointF(171.402358464443f, 159.37469513797f), new PointF(162.724939736444f, 188.029175232746f) },</v>
       </c>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
       <c r="F116" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G116" s="8" t="str">
+      <c r="G116" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H121, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H122, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H123, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H124, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H125, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H126, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H127, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H128, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (724.447298414639f, 143.245187883143f), new PointF(732.249000465397f, 116.723494587481f), new PointF(738.732781042897f, 116.924565396825f), new PointF(731.175992417625f, 148.948115406062f) },</v>
       </c>
-      <c r="H116" s="8"/>
-      <c r="I116" s="8"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7"/>
       <c r="K116" s="2"/>
       <c r="M116"/>
       <c r="Q116" s="2"/>
@@ -4188,7 +4263,7 @@
       <c r="A130" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B130" s="8" t="str">
+      <c r="B130" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
 SUBSTITUTE(TEXT(C135, "0,00"), ",", ".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(C136, "0,00"), ",", ".") &amp; "f), new PointF(" &amp;
@@ -4200,12 +4275,12 @@
 SUBSTITUTE(TEXT(C142, "0,00"), ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (120.43f, 215.63f), new PointF(128.50f, 211.51f), new PointF(132.29f, 218.01f), new PointF(124.24f, 222.78f) },</v>
       </c>
-      <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
+      <c r="C130" s="7"/>
+      <c r="D130" s="7"/>
       <c r="F130" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G130" s="8" t="str">
+      <c r="G130" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
 SUBSTITUTE(TEXT(H135, "0,00"), ",", ".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(H136, "0,00"), ",", ".") &amp; "f), new PointF(" &amp;
@@ -4217,8 +4292,8 @@
 SUBSTITUTE(TEXT(H142, "0,00"), ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (685.45f, 173.13f), new PointF(693.84f, 170.15f), new PointF(694.65f, 177.28f), new PointF(686.09f, 180.39f) },</v>
       </c>
-      <c r="H130" s="8"/>
-      <c r="I130" s="8"/>
+      <c r="H130" s="7"/>
+      <c r="I130" s="7"/>
       <c r="K130" s="2"/>
       <c r="M130"/>
       <c r="Q130" s="2"/>
@@ -4531,7 +4606,7 @@
       <c r="A144" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B144" s="8" t="str">
+      <c r="B144" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
 SUBSTITUTE(TEXT(C149, "0,00"), ",", ".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(C150, "0,00"), ",", ".") &amp; "f), new PointF(" &amp;
@@ -4543,12 +4618,12 @@
 SUBSTITUTE(TEXT(C156, "0,00"), ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (92.00f, 111.85f), new PointF(72.65f, 125.87f), new PointF(64.69f, 117.36f), new PointF(87.98f, 102.65f) },</v>
       </c>
-      <c r="C144" s="8"/>
-      <c r="D144" s="8"/>
+      <c r="C144" s="7"/>
+      <c r="D144" s="7"/>
       <c r="F144" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="G144" s="8" t="str">
+      <c r="G144" s="7" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
 SUBSTITUTE(TEXT(H149, "0,00"), ",", ".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(H150, "0,00"), ",", ".") &amp; "f), new PointF(" &amp;
@@ -4560,8 +4635,8 @@
 SUBSTITUTE(TEXT(H156, "0,00"), ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (655.93f, 71.53f), new PointF(640.17f, 86.63f), new PointF(629.79f, 80.02f), new PointF(649.91f, 63.27f) },</v>
       </c>
-      <c r="H144" s="8"/>
-      <c r="I144" s="8"/>
+      <c r="H144" s="7"/>
+      <c r="I144" s="7"/>
       <c r="K144" s="2"/>
       <c r="M144"/>
       <c r="Q144" s="2"/>
@@ -4889,30 +4964,30 @@
       <c r="A161" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B161" s="8" t="str">
+      <c r="B161" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(C162,",",".") &amp; "f, " &amp; SUBSTITUTE(C163,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(C164,",",".") &amp; "f, " &amp; SUBSTITUTE(C165,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(C166,",",".") &amp; "f, " &amp; SUBSTITUTE(C167,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(C168,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(78.7676348023617f, 197.045802607026f), PixelSize1 = new SizeF(3.75987462459764f, 5.14884893927504f), PixelSize2 = new SizeF(6.62400107264758f, 9.12188718706622f), Degrees = 40f },</v>
       </c>
-      <c r="C161" s="8"/>
-      <c r="D161" s="8"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="7"/>
       <c r="F161" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G161" s="8" t="str">
+      <c r="G161" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(H162,",",".") &amp; "f, " &amp; SUBSTITUTE(H163,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(H164,",",".") &amp; "f, " &amp; SUBSTITUTE(H165,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(H166,",",".") &amp; "f, " &amp; SUBSTITUTE(H167,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(H168,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(645.372198995559f, 151.289343091178f), PixelSize1 = new SizeF(4.38803220663234f, 5.85486448787416f), PixelSize2 = new SizeF(6.98456806016931f, 8.64037551205804f), Degrees = 60f },</v>
       </c>
-      <c r="H161" s="8"/>
-      <c r="I161" s="8"/>
+      <c r="H161" s="7"/>
+      <c r="I161" s="7"/>
       <c r="K161" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L161" s="8" t="str">
+      <c r="L161" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(M162,",",".") &amp; "f, " &amp; SUBSTITUTE(M163,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(M164,",",".") &amp; "f, " &amp; SUBSTITUTE(M165,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(M166,",",".") &amp; "f, " &amp; SUBSTITUTE(M167,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(M168,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(262.575160629947f, 583.607457192202f), PixelSize1 = new SizeF(5.80724503487562f, 11.4602802273139f), PixelSize2 = new SizeF(6.62400107264758f, 9.12188718706622f), Degrees = 70f },</v>
       </c>
-      <c r="M161" s="8"/>
-      <c r="N161" s="8"/>
+      <c r="M161" s="7"/>
+      <c r="N161" s="7"/>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
@@ -5210,30 +5285,30 @@
       <c r="A170" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B170" s="8" t="str">
+      <c r="B170" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(C171,",",".") &amp; "f, " &amp; SUBSTITUTE(C172,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(C173,",",".") &amp; "f, " &amp; SUBSTITUTE(C174,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(C175,",",".") &amp; "f, " &amp; SUBSTITUTE(C176,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(C177,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(89.3994475476303f, 168.448015409621f), PixelSize1 = new SizeF(11.1730411793682f, 10.7433040518897f), PixelSize2 = new SizeF(13.9683802147044f, 13.8644370285125f), Degrees = 60f },</v>
       </c>
-      <c r="C170" s="8"/>
-      <c r="D170" s="8"/>
+      <c r="C170" s="7"/>
+      <c r="D170" s="7"/>
       <c r="F170" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G170" s="8" t="str">
+      <c r="G170" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(H171,",",".") &amp; "f, " &amp; SUBSTITUTE(H172,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(H173,",",".") &amp; "f, " &amp; SUBSTITUTE(H174,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(H175,",",".") &amp; "f, " &amp; SUBSTITUTE(H176,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(H177,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(655.591287264545f, 125.473287391466f), PixelSize1 = new SizeF(10.0267102850775f, 9.31539894342744f), PixelSize2 = new SizeF(12.8326319992927f, 12.1194296474193f), Degrees = 62.1f },</v>
       </c>
-      <c r="H170" s="8"/>
-      <c r="I170" s="8"/>
+      <c r="H170" s="7"/>
+      <c r="I170" s="7"/>
       <c r="K170" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="L170" s="8" t="str">
+      <c r="L170" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(M171,",",".") &amp; "f, " &amp; SUBSTITUTE(M172,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(M173,",",".") &amp; "f, " &amp; SUBSTITUTE(M174,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(M175,",",".") &amp; "f, " &amp; SUBSTITUTE(M176,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(M177,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(274.061146741882f, 554.067056087834f), PixelSize1 = new SizeF(11.9108050783645f, 13.9702637702726f), PixelSize2 = new SizeF(6.62400107264758f, 9.12188718706622f), Degrees = 59.9f },</v>
       </c>
-      <c r="M170" s="8"/>
-      <c r="N170" s="8"/>
+      <c r="M170" s="7"/>
+      <c r="N170" s="7"/>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
@@ -5531,30 +5606,30 @@
       <c r="A179" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B179" s="8" t="str">
+      <c r="B179" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(C180,",",".") &amp; "f, " &amp; SUBSTITUTE(C181,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(C182,",",".") &amp; "f, " &amp; SUBSTITUTE(C183,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(C184,",",".") &amp; "f, " &amp; SUBSTITUTE(C185,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(C186,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(120.313342317405f, 129.814829472171f), PixelSize1 = new SizeF(7.31716653922499f, 8.84106836875298f), PixelSize2 = new SizeF(9.9715291737796f, 11.56346130053f), Degrees = 75f },</v>
       </c>
-      <c r="C179" s="8"/>
-      <c r="D179" s="8"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="7"/>
       <c r="F179" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G179" s="8" t="str">
+      <c r="G179" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(H180,",",".") &amp; "f, " &amp; SUBSTITUTE(H181,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(H182,",",".") &amp; "f, " &amp; SUBSTITUTE(H183,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(H184,",",".") &amp; "f, " &amp; SUBSTITUTE(H185,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(H186,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(683.08659880357f, 85.4726687694167f), PixelSize1 = new SizeF(8.2223635362004f, 10.2194616801775f), PixelSize2 = new SizeF(10.3714032542806f, 12.3594295796251f), Degrees = 80f },</v>
       </c>
-      <c r="H179" s="8"/>
-      <c r="I179" s="8"/>
+      <c r="H179" s="7"/>
+      <c r="I179" s="7"/>
       <c r="K179" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="L179" s="8" t="str">
+      <c r="L179" s="7" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(M180,",",".") &amp; "f, " &amp; SUBSTITUTE(M181,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(M182,",",".") &amp; "f, " &amp; SUBSTITUTE(M183,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(M184,",",".") &amp; "f, " &amp; SUBSTITUTE(M185,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(M186,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(303.938694887144f, 517.110846054632f), PixelSize1 = new SizeF(7.20302478845816f, 12.9161538318128f), PixelSize2 = new SizeF(6.62400107264758f, 9.12188718706622f), Degrees = 70f },</v>
       </c>
-      <c r="M179" s="8"/>
-      <c r="N179" s="8"/>
+      <c r="M179" s="7"/>
+      <c r="N179" s="7"/>
     </row>
     <row r="180" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
@@ -5869,39 +5944,39 @@
       <c r="A190" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B190" s="8" t="str">
+      <c r="B190" s="7" t="str">
         <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(C191,",",".")&amp;"f, "&amp;SUBSTITUTE(C192,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(C193,",",".")&amp;"f, "&amp;SUBSTITUTE(C194,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(C195,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(C196,",",".")&amp;"f, "&amp;SUBSTITUTE(C197,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(C198,",",".")&amp;"f, "&amp;SUBSTITUTE(C199,",",".")&amp;"f) },"</f>
         <v>new Number { PixelCenter = new PointF(124.723673740246f, 175.531981912508f), PixelSize = new SizeF(90.681085550446f, 95.4390911509929f), Degrees = -24f, OrientStart = new PointF(138.7196445106f, 156.106349604506f), OrientEnd = new PointF(127.381059997338f, 201.460667501665f) },</v>
       </c>
-      <c r="C190" s="8"/>
-      <c r="D190" s="8"/>
+      <c r="C190" s="7"/>
+      <c r="D190" s="7"/>
       <c r="F190" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G190" s="8" t="str">
+      <c r="G190" s="7" t="str">
         <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(H191,",",".")&amp;"f, "&amp;SUBSTITUTE(H192,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(H193,",",".")&amp;"f, "&amp;SUBSTITUTE(H194,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(H195,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(H196,",",".")&amp;"f, "&amp;SUBSTITUTE(H197,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(H198,",",".")&amp;"f, "&amp;SUBSTITUTE(H199,",",".")&amp;"f) },"</f>
         <v>new Number { PixelCenter = new PointF(641.059001446714f, 154.743074399047f), PixelSize = new SizeF(74.1679490181485f, 93.615469618878f), Degrees = 41.3f, OrientStart = new PointF(644.949647746031f, 184.830750939373f), OrientEnd = new PointF(653.944924793219f, 144.578793805644f) },</v>
       </c>
-      <c r="H190" s="8"/>
-      <c r="I190" s="8"/>
+      <c r="H190" s="7"/>
+      <c r="I190" s="7"/>
       <c r="K190" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="L190" s="8" t="str">
+      <c r="L190" s="7" t="str">
         <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(M191,",",".")&amp;"f, "&amp;SUBSTITUTE(M192,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(M193,",",".")&amp;"f, "&amp;SUBSTITUTE(M194,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(M195,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(M196,",",".")&amp;"f, "&amp;SUBSTITUTE(M197,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(M198,",",".")&amp;"f, "&amp;SUBSTITUTE(M199,",",".")&amp;"f) },"</f>
         <v>new Number { PixelCenter = new PointF(520.968651291404f, 181.078059086033f), PixelSize = new SizeF(98.2144411010572f, 93.1022099213418f), Degrees = 96f, OrientStart = new PointF(510.133877883348f, 199.192951606807f), OrientEnd = new PointF(534.889787403969f, 163.287449938223f) },</v>
       </c>
-      <c r="M190" s="8"/>
-      <c r="N190" s="8"/>
+      <c r="M190" s="7"/>
+      <c r="N190" s="7"/>
       <c r="P190" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Q190" s="8" t="str">
+      <c r="Q190" s="7" t="str">
         <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(R191,",",".")&amp;"f, "&amp;SUBSTITUTE(R192,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(R193,",",".")&amp;"f, "&amp;SUBSTITUTE(R194,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(R195,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(R196,",",".")&amp;"f, "&amp;SUBSTITUTE(R197,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(R198,",",".")&amp;"f, "&amp;SUBSTITUTE(R199,",",".")&amp;"f) },"</f>
         <v>new Number { PixelCenter = new PointF(486.888267819892f, 205.256068004359f), PixelSize = new SizeF(92.5296527789248f, 94.4443197784486f), Degrees = -4.8f, OrientStart = new PointF(473.283478215247f, 225.271684397674f), OrientEnd = new PointF(498.228364144423f, 189.744135378232f) },</v>
       </c>
-      <c r="R190" s="8"/>
-      <c r="S190" s="8"/>
+      <c r="R190" s="7"/>
+      <c r="S190" s="7"/>
     </row>
     <row r="191" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
@@ -6389,8 +6464,456 @@
         <v>6</v>
       </c>
     </row>
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B201"/>
+      <c r="F201" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="K201" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="M201"/>
+    </row>
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B202"/>
+      <c r="M202"/>
+    </row>
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B203" s="7" t="str">
+        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(C204,",",".")&amp;"f, "&amp;SUBSTITUTE(C205,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(C206,",",".")&amp;"f, "&amp;SUBSTITUTE(C207,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(C208,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(C209,",",".")&amp;"f, "&amp;SUBSTITUTE(C210,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(C211,",",".")&amp;"f, "&amp;SUBSTITUTE(C212,",",".")&amp;"f) },"</f>
+        <v>new Number { PixelCenter = new PointF(288.97025151837f, 209.327373940928f), PixelSize = new SizeF(90.708676106095f, 57.5992278240944f), Degrees = 41f, OrientStart = new PointF(302.259828473547f, 220.736252607958f), OrientEnd = new PointF(282.606281983893f, 189.366182729089f) },</v>
+      </c>
+      <c r="C203" s="7"/>
+      <c r="D203" s="7"/>
+      <c r="F203" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G203" s="7" t="str">
+        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(H204,",",".")&amp;"f, "&amp;SUBSTITUTE(H205,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(H206,",",".")&amp;"f, "&amp;SUBSTITUTE(H207,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(H208,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(H209,",",".")&amp;"f, "&amp;SUBSTITUTE(H210,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(H211,",",".")&amp;"f, "&amp;SUBSTITUTE(H212,",",".")&amp;"f) },"</f>
+        <v>new Number { PixelCenter = new PointF(324.389721820897f, 264.19778363821f), PixelSize = new SizeF(90.708676106095f, 90.7086357943192f), Degrees = 30f, OrientStart = new PointF(340.527551205805f, 259.948839956544f), OrientEnd = new PointF(320.212587286211f, 224.515779099388f) },</v>
+      </c>
+      <c r="H203" s="7"/>
+      <c r="I203" s="7"/>
+      <c r="K203" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L203" s="7" t="str">
+        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(M204,",",".")&amp;"f, "&amp;SUBSTITUTE(M205,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(M206,",",".")&amp;"f, "&amp;SUBSTITUTE(M207,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(M208,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(M209,",",".")&amp;"f, "&amp;SUBSTITUTE(M210,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(M211,",",".")&amp;"f, "&amp;SUBSTITUTE(M212,",",".")&amp;"f) },"</f>
+        <v>new Number { PixelCenter = new PointF(332.014164000431f, 279.4833226275f), PixelSize = new SizeF(90.708676106095f, 90.7086357943192f), Degrees = 41f, OrientStart = new PointF(324.93699750007f, 301.996072173702f), OrientEnd = new PointF(334.291329723511f, 262.783484825116f) },</v>
+      </c>
+      <c r="M203" s="7"/>
+      <c r="N203" s="7"/>
+    </row>
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>10</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C204">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B204,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>288.97025151836959</v>
+      </c>
+      <c r="D204" t="s">
+        <v>6</v>
+      </c>
+      <c r="F204" t="s">
+        <v>10</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="H204">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G204,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>324.38972182089697</v>
+      </c>
+      <c r="I204" t="s">
+        <v>6</v>
+      </c>
+      <c r="K204" t="s">
+        <v>10</v>
+      </c>
+      <c r="L204" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="M204">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L204,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>332.01416400043138</v>
+      </c>
+      <c r="N204" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>11</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C205">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B205,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>209.3273739409276</v>
+      </c>
+      <c r="D205" t="s">
+        <v>6</v>
+      </c>
+      <c r="F205" t="s">
+        <v>11</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="H205">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G205,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>264.1977836382095</v>
+      </c>
+      <c r="I205" t="s">
+        <v>6</v>
+      </c>
+      <c r="K205" t="s">
+        <v>11</v>
+      </c>
+      <c r="L205" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="M205">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L205,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>279.48332262749966</v>
+      </c>
+      <c r="N205" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>4</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C206">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B206,".",",")," mm",""))*$B$2/$B$6</f>
+        <v>90.708676106094956</v>
+      </c>
+      <c r="D206" t="s">
+        <v>6</v>
+      </c>
+      <c r="F206" t="s">
+        <v>4</v>
+      </c>
+      <c r="G206" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H206">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G206,".",",")," mm",""))*$B$2/$B$6</f>
+        <v>90.708676106094956</v>
+      </c>
+      <c r="I206" t="s">
+        <v>6</v>
+      </c>
+      <c r="K206" t="s">
+        <v>4</v>
+      </c>
+      <c r="L206" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="M206">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L206,".",",")," mm",""))*$B$2/$B$6</f>
+        <v>90.708676106094956</v>
+      </c>
+      <c r="N206" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>5</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C207">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B207,".",",")," mm",""))*$B$3/$B$7</f>
+        <v>57.599227824094392</v>
+      </c>
+      <c r="D207" t="s">
+        <v>6</v>
+      </c>
+      <c r="F207" t="s">
+        <v>5</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H207">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G207,".",",")," mm",""))*$B$3/$B$7</f>
+        <v>90.708635794319179</v>
+      </c>
+      <c r="I207" t="s">
+        <v>6</v>
+      </c>
+      <c r="K207" t="s">
+        <v>5</v>
+      </c>
+      <c r="L207" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="M207">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L207,".",",")," mm",""))*$B$3/$B$7</f>
+        <v>90.708635794319179</v>
+      </c>
+      <c r="N207" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>141</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C208">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B208,".",",")," deg",""))</f>
+        <v>41</v>
+      </c>
+      <c r="D208" t="s">
+        <v>161</v>
+      </c>
+      <c r="F208" t="s">
+        <v>141</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="H208">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G208,".",",")," deg",""))</f>
+        <v>30</v>
+      </c>
+      <c r="I208" t="s">
+        <v>161</v>
+      </c>
+      <c r="K208" t="s">
+        <v>141</v>
+      </c>
+      <c r="L208" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="M208">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L208,".",",")," deg",""))</f>
+        <v>41</v>
+      </c>
+      <c r="N208" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>195</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C209">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B209,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>302.25982847354669</v>
+      </c>
+      <c r="D209" t="s">
+        <v>6</v>
+      </c>
+      <c r="F209" t="s">
+        <v>195</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="H209">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G209,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>340.52755120580548</v>
+      </c>
+      <c r="I209" t="s">
+        <v>6</v>
+      </c>
+      <c r="K209" t="s">
+        <v>195</v>
+      </c>
+      <c r="L209" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="M209">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L209,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>324.93699750007039</v>
+      </c>
+      <c r="N209" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>196</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C210">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B210,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>220.73625260795802</v>
+      </c>
+      <c r="D210" t="s">
+        <v>6</v>
+      </c>
+      <c r="F210" t="s">
+        <v>196</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="H210">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G210,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>259.94883995654396</v>
+      </c>
+      <c r="I210" t="s">
+        <v>6</v>
+      </c>
+      <c r="K210" t="s">
+        <v>196</v>
+      </c>
+      <c r="L210" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="M210">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L210,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>301.99607217370232</v>
+      </c>
+      <c r="N210" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>197</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C211">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B211,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>282.60628198389276</v>
+      </c>
+      <c r="D211" t="s">
+        <v>6</v>
+      </c>
+      <c r="F211" t="s">
+        <v>197</v>
+      </c>
+      <c r="G211" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="H211">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G211,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>320.21258728621132</v>
+      </c>
+      <c r="I211" t="s">
+        <v>6</v>
+      </c>
+      <c r="K211" t="s">
+        <v>197</v>
+      </c>
+      <c r="L211" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="M211">
+        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L211,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
+        <v>334.29132972351147</v>
+      </c>
+      <c r="N211" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>198</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C212">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B212,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>189.36618272908925</v>
+      </c>
+      <c r="D212" t="s">
+        <v>6</v>
+      </c>
+      <c r="F212" t="s">
+        <v>198</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="H212">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G212,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>224.515779099388</v>
+      </c>
+      <c r="I212" t="s">
+        <v>6</v>
+      </c>
+      <c r="K212" t="s">
+        <v>198</v>
+      </c>
+      <c r="L212" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="M212">
+        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L212,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
+        <v>262.78348482511643</v>
+      </c>
+      <c r="N212" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="49">
+    <mergeCell ref="B203:D203"/>
+    <mergeCell ref="G203:I203"/>
+    <mergeCell ref="L203:N203"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="B179:D179"/>
+    <mergeCell ref="G161:I161"/>
+    <mergeCell ref="G170:I170"/>
+    <mergeCell ref="G179:I179"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="G116:I116"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="B46:D46"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B144:D144"/>
     <mergeCell ref="G144:I144"/>
@@ -6407,36 +6930,6 @@
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="G88:I88"/>
     <mergeCell ref="G74:I74"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="B179:D179"/>
-    <mergeCell ref="G161:I161"/>
-    <mergeCell ref="G170:I170"/>
-    <mergeCell ref="G179:I179"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="G116:I116"/>
-    <mergeCell ref="G102:I102"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
WIP on time-dependent ball positions/-orientations (for motion blur). Improved GUI (added view-options)
</commit_message>
<xml_diff>
--- a/Documentation/Original.xlsx
+++ b/Documentation/Original.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="375">
   <si>
     <t>Pixelwidth</t>
   </si>
@@ -518,9 +518,6 @@
     <t>47 mm</t>
   </si>
   <si>
-    <t>Ball w</t>
-  </si>
-  <si>
     <t>Ball 1</t>
   </si>
   <si>
@@ -539,9 +536,6 @@
     <t>Ball 8b</t>
   </si>
   <si>
-    <t>Ball 4</t>
-  </si>
-  <si>
     <t>Boxes on Ball 1</t>
   </si>
   <si>
@@ -560,9 +554,6 @@
     <t>133,35 mm</t>
   </si>
   <si>
-    <t>Number on Ball 1</t>
-  </si>
-  <si>
     <t>35.2769 mm</t>
   </si>
   <si>
@@ -578,12 +569,6 @@
     <t>-24.0000 deg</t>
   </si>
   <si>
-    <t>Number1</t>
-  </si>
-  <si>
-    <t>Number on Ball 4</t>
-  </si>
-  <si>
     <t>19.6236 mm</t>
   </si>
   <si>
@@ -650,24 +635,9 @@
     <t>-4.8000 deg</t>
   </si>
   <si>
-    <t>127,5 mm</t>
-  </si>
-  <si>
-    <t>177,3 mm</t>
-  </si>
-  <si>
-    <t>134,1 mm</t>
-  </si>
-  <si>
     <t>186,7 mm</t>
   </si>
   <si>
-    <t>Number on Ball 8a</t>
-  </si>
-  <si>
-    <t>Number on Ball 8b</t>
-  </si>
-  <si>
     <t>137,25 mm</t>
   </si>
   <si>
@@ -758,15 +728,6 @@
     <t>185,8214 mm</t>
   </si>
   <si>
-    <t>80,7246 mm</t>
-  </si>
-  <si>
-    <t>91,2058 mm</t>
-  </si>
-  <si>
-    <t>-19 deg</t>
-  </si>
-  <si>
     <t>23,1177 mm</t>
   </si>
   <si>
@@ -1073,15 +1034,6 @@
     <t>194,8 mm</t>
   </si>
   <si>
-    <t>Number on Ball 9a</t>
-  </si>
-  <si>
-    <t>Number on Ball 9b</t>
-  </si>
-  <si>
-    <t>Number on Ball 9c</t>
-  </si>
-  <si>
     <t>78,7338 mm</t>
   </si>
   <si>
@@ -1146,6 +1098,57 @@
   </si>
   <si>
     <t>167,375 mm</t>
+  </si>
+  <si>
+    <t>Ball 4a</t>
+  </si>
+  <si>
+    <t>Ball 4b</t>
+  </si>
+  <si>
+    <t>-179,7 deg</t>
+  </si>
+  <si>
+    <t>188,5597 mm</t>
+  </si>
+  <si>
+    <t>208,5115 mm</t>
+  </si>
+  <si>
+    <t>179,5409 mm</t>
+  </si>
+  <si>
+    <t>200,0604 mm</t>
+  </si>
+  <si>
+    <t>180,5703 mm</t>
+  </si>
+  <si>
+    <t>192,0997 mm</t>
+  </si>
+  <si>
+    <t>182,9503 mm</t>
+  </si>
+  <si>
+    <t>Ball wa</t>
+  </si>
+  <si>
+    <t>Ball wb</t>
+  </si>
+  <si>
+    <t>80,375 mm</t>
+  </si>
+  <si>
+    <t>91,25 mm</t>
+  </si>
+  <si>
+    <t>0 deg</t>
+  </si>
+  <si>
+    <t>78,375 mm</t>
+  </si>
+  <si>
+    <t>91,875 mm</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1206,6 +1209,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1494,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U212"/>
+  <dimension ref="A1:U238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G182" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L214" sqref="L214"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1527,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1538,20 +1544,20 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="G2" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="H2" t="s">
-        <v>309</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+        <v>296</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="5" t="str">
         <f>"new ColorRef { PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F2,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
@@ -1576,20 +1582,20 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="G3" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="H3" t="s">
-        <v>310</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+        <v>297</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="5" t="str">
         <f t="shared" ref="M3:M12" si="0">"new ColorRef { PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F3,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
@@ -1612,20 +1618,20 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="G4" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="H4" t="s">
-        <v>313</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+        <v>300</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(86.20f, 287.82f), Radius = 35.91f }, // Cloth with shadow of lamp 1 (highest)</v>
@@ -1645,20 +1651,20 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
+        <v>301</v>
+      </c>
+      <c r="G5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="G5" t="s">
-        <v>315</v>
-      </c>
-      <c r="H5" t="s">
-        <v>316</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
       <c r="M5" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(398.50f, 575.20f), Radius = 20.52f }, // Cloth with shadow of lamp 2</v>
@@ -1678,20 +1684,20 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="G6" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="H6" t="s">
-        <v>319</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+        <v>306</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(444.56f, 449.02f), Radius = 30.99f }, // Cloth with shadow of lamp 3 (lowest)</v>
@@ -1711,20 +1717,20 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="G7" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="H7" t="s">
-        <v>322</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+        <v>309</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(83.24f, 134.94f), Radius = 20.41f }, // Lightest part of Ball 1</v>
@@ -1735,20 +1741,20 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="G8" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="H8" t="s">
-        <v>322</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+        <v>309</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>new ColorRef { PixelCenter = new PointF(709.32f, 99.04f), Radius = 20.41f }, // Lightest part of Ball 4</v>
@@ -1756,9 +1762,157 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>321</v>
+      </c>
+      <c r="G9" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" t="s">
+        <v>309</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new ColorRef { PixelCenter = new PointF(304.50f, 545.56f), Radius = 20.41f }, // Lightest part of Ball w</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>324</v>
+      </c>
+      <c r="G10" t="s">
+        <v>325</v>
+      </c>
+      <c r="H10" t="s">
+        <v>326</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new ColorRef { PixelCenter = new PointF(621.44f, 73.33f), Radius = 18.90f }, // Reflection of cloth in Ball 4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>328</v>
+      </c>
+      <c r="G11" t="s">
+        <v>329</v>
+      </c>
+      <c r="H11" t="s">
+        <v>330</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new ColorRef { PixelCenter = new PointF(111.02f, 169.15f), Radius = 12.47f }, // White part of the number texture</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>334</v>
+      </c>
+      <c r="G12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H12" t="s">
+        <v>331</v>
+      </c>
+      <c r="I12" t="s">
+        <v>333</v>
+      </c>
+      <c r="M12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new ColorRef { PixelCenter = new PointF(132.75f, 159.13f), Radius = 8.31f }, // Black part of the number texture</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="7" t="str">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5" t="str">
         <f>"new Ball { Name = """ &amp; A9 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B10,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B11,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -1767,139 +1921,29 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B14,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 1", PixelCenter = new PointF(111.78f, 166.22f), PixelSize = new SizeF(175.02f, 176.32f), Degrees = -179.50f },</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G9" t="s">
-        <v>335</v>
-      </c>
-      <c r="H9" t="s">
-        <v>322</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new ColorRef { PixelCenter = new PointF(304.50f, 545.56f), Radius = 20.41f }, // Lightest part of Ball w</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="Q16" s="2"/>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>337</v>
-      </c>
-      <c r="G10" t="s">
-        <v>338</v>
-      </c>
-      <c r="H10" t="s">
-        <v>339</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new ColorRef { PixelCenter = new PointF(621.44f, 73.33f), Radius = 18.90f }, // Reflection of cloth in Ball 4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>222</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
         <v>224</v>
       </c>
-      <c r="E11">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>341</v>
-      </c>
-      <c r="G11" t="s">
-        <v>342</v>
-      </c>
-      <c r="H11" t="s">
-        <v>343</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new ColorRef { PixelCenter = new PointF(111.02f, 169.15f), Radius = 12.47f }, // White part of the number texture</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>347</v>
-      </c>
-      <c r="G12" t="s">
-        <v>348</v>
-      </c>
-      <c r="H12" t="s">
-        <v>344</v>
-      </c>
-      <c r="I12" t="s">
-        <v>346</v>
-      </c>
-      <c r="M12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>new ColorRef { PixelCenter = new PointF(132.75f, 159.13f), Radius = 8.31f }, // Black part of the number texture</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B16" s="7" t="str">
+      <c r="M17" s="5" t="str">
         <f>"new Ball { Name = """ &amp; A16 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -1908,77 +1952,34 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 9a", PixelCenter = new PointF(326.64f, 247.57f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16" s="7" t="str">
-        <f>"new Ball { Name = """ &amp; E16 &amp; """, PixelCenter = new PointF(" &amp;
-SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
-SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(F18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(F19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(F20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(F21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 9b", PixelCenter = new PointF(337.32f, 267.88f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="J16" s="7" t="str">
-        <f>"new Ball { Name = """ &amp; I16 &amp; """, PixelCenter = new PointF(" &amp;
-SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(J17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
-SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(J18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(J19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(J20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(J21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 9c", PixelCenter = new PointF(340.62f, 297.17f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="Q16" s="2"/>
-      <c r="U16" s="2"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>232</v>
-      </c>
-      <c r="I17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" t="s">
-        <v>234</v>
-      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>229</v>
+        <v>219</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
       </c>
       <c r="E18" t="s">
+        <v>223</v>
+      </c>
+      <c r="G18" t="s">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
-        <v>233</v>
-      </c>
-      <c r="I18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" t="s">
-        <v>235</v>
+      <c r="H18" t="s">
+        <v>225</v>
+      </c>
+      <c r="M18" s="5" t="str">
+        <f>"new Ball { Name = """ &amp; D16 &amp; """, PixelCenter = new PointF(" &amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
+        <v>new Ball { Name = "Ball 9b", PixelCenter = new PointF(337.32f, 267.88f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1986,19 +1987,28 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>230</v>
+        <v>220</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
       </c>
       <c r="E19" t="s">
+        <v>220</v>
+      </c>
+      <c r="G19" t="s">
         <v>4</v>
       </c>
-      <c r="F19" t="s">
-        <v>230</v>
-      </c>
-      <c r="I19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" t="s">
-        <v>230</v>
+      <c r="H19" t="s">
+        <v>220</v>
+      </c>
+      <c r="M19" s="5" t="str">
+        <f>"new Ball { Name = """ &amp; G16 &amp; """, PixelCenter = new PointF(" &amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(H17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(H18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
+        <v>new Ball { Name = "Ball 9c", PixelCenter = new PointF(340.62f, 297.17f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2006,46 +2016,21 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>231</v>
+        <v>221</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
       </c>
       <c r="E20" t="s">
+        <v>221</v>
+      </c>
+      <c r="G20" t="s">
         <v>5</v>
       </c>
-      <c r="F20" t="s">
-        <v>231</v>
-      </c>
-      <c r="I20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="E21" t="s">
-        <v>141</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="I21" t="s">
-        <v>141</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" s="7" t="str">
+      <c r="H20" t="s">
+        <v>221</v>
+      </c>
+      <c r="M20" s="5" t="str">
         <f>"new Ball { Name = """ &amp; A23 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B24,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B25,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
@@ -2054,175 +2039,289 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 8a", PixelCenter = new PointF(513.15f, 187.86f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F23" s="7" t="str">
-        <f>"new Ball { Name = """ &amp; E23 &amp; """, PixelCenter = new PointF(" &amp;
-SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F24,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
-SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(F25,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(F26,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(F27,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
-SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(F28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G21" t="s">
+        <v>141</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="M21" s="5" t="str">
+        <f>"new Ball { Name = """ &amp; D23 &amp; """, PixelCenter = new PointF(" &amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E24,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E25,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E26,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E27,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
         <v>new Ball { Name = "Ball 8b", PixelCenter = new PointF(495.39f, 193.06f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E24" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E25" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="E26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="E28" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B30" s="7" t="str">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M22" s="5" t="str">
         <f>"new Ball { Name = """ &amp; A30 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B31,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B32,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B33,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B34,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B35,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 4", PixelCenter = new PointF(675.32f, 122.76f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+        <v>new Ball { Name = "Ball 4a", PixelCenter = new PointF(675.32f, 122.76f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = -179.70f },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="M23" s="5" t="str">
+        <f>"new Ball { Name = """ &amp; D30 &amp; """, PixelCenter = new PointF(" &amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E31,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E32,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E33,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E34,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E35,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
+        <v>new Ball { Name = "Ball 4b", PixelCenter = new PointF(704.06f, 107.31f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = -179.70f },</v>
+      </c>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>141</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B37" s="7" t="str">
+      <c r="B24" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>175</v>
+      </c>
+      <c r="M24" s="5" t="str">
         <f>"new Ball { Name = """ &amp; A37 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B38,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B39,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B40,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B41,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B42,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball w", PixelCenter = new PointF(296.49f, 550.67f), PixelSize = new SizeF(177.64f, 177.64f), Degrees = -19.00f },</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+        <v>new Ball { Name = "Ball wa", PixelCenter = new PointF(295.17f, 550.50f), PixelSize = new SizeF(177.64f, 177.64f), Degrees = 0.00f },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>233</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="5" t="str">
+        <f>"new Ball { Name = """ &amp; D37 &amp; """, PixelCenter = new PointF(" &amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E38,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E39,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E40,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E41,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E42,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
+        <v>new Ball { Name = "Ball wb", PixelCenter = new PointF(287.61f, 548.14f), PixelSize = new SizeF(177.64f, 177.64f), Degrees = 0.00f },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="L28" s="2"/>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L29" s="2"/>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="L30" s="2"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="L32" s="2"/>
+      <c r="M32"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D35" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="I35" s="4"/>
+      <c r="L35" s="2"/>
+      <c r="M35"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>244</v>
+        <v>370</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2230,7 +2329,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>245</v>
+        <v>371</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2240,6 +2345,12 @@
       <c r="B40" s="3" t="s">
         <v>163</v>
       </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -2248,23 +2359,35 @@
       <c r="B41" s="3" t="s">
         <v>163</v>
       </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>141</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>246</v>
+        <v>372</v>
+      </c>
+      <c r="D42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>372</v>
       </c>
       <c r="F42" s="4"/>
       <c r="J42" s="4"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K44" s="2"/>
       <c r="M44"/>
@@ -2277,21 +2400,21 @@
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="7" t="str">
+      <c r="B46" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C51, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C52, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C53, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C54, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C55, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C56, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C57, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C58, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (133.742761814912f, 205.892540265516f), new PointF(137.83334515448f, 202.417265656646f), new PointF(140.168715611395f, 205.047438142032f), new PointF(136.177533862726f, 208.63383082975f) },</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
       <c r="F46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G46" s="7" t="str">
+      <c r="G46" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H51, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H52, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H53, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H54, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H55, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H56, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H57, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H58, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (699.875451915949f, 164.6093393286f), new PointF(703.879106107581f, 161.802662956064f), new PointF(705.755263891709f, 165.080646282082f), new PointF(700.908774917924f, 168.021873797712f) },</v>
       </c>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
       <c r="K46" s="2"/>
       <c r="M46"/>
       <c r="Q46" s="2"/>
@@ -2608,21 +2731,21 @@
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="7" t="str">
+      <c r="B60" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C65, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C66, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C67, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C68, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C69, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C70, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C71, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C72, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (138.596053939405f, 201.709927273775f), new PointF(149.288339135411f, 188.969143471165f), new PointF(152.571237304817f, 191.438686080665f), new PointF(140.923865339978f, 204.331028895582f) },</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
       <c r="F60" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G60" s="7" t="str">
+      <c r="G60" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H65, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H66, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H67, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H68, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H69, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H70, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H71, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H72, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (704.847421225014f, 161.05715135563f), new PointF(717.414352393879f, 148.062005420146f), new PointF(720.371077282121f, 151.265154121633f), new PointF(706.79312232749f, 164.366882704175f) },</v>
       </c>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
       <c r="K60" s="2"/>
       <c r="M60"/>
       <c r="Q60" s="2"/>
@@ -2939,21 +3062,21 @@
       <c r="A74" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B74" s="7" t="str">
+      <c r="B74" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C79, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C80, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C81, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C82, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C83, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C84, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C85, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C86, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (149.881725058272f, 188.044293338712f), new PointF(152.033788398889f, 184.38004240527f), new PointF(156.288025308265f, 186.401333172887f), new PointF(153.240969696734f, 190.571284750882f) },</v>
       </c>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
       <c r="F74" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G74" s="7" t="str">
+      <c r="G74" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H79, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H80, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H81, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H82, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H83, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H84, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H85, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H86, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (718.239423393628f, 146.901312834628f), new PointF(721.061219126161f, 142.460369207198f), new PointF(724.375487379388f, 145.268935342979f), new PointF(721.251707345984f, 150.072335560938f) },</v>
       </c>
-      <c r="H74" s="7"/>
-      <c r="I74" s="7"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
       <c r="K74" s="2"/>
       <c r="M74"/>
       <c r="Q74" s="2"/>
@@ -3270,21 +3393,21 @@
       <c r="A88" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B88" s="7" t="str">
+      <c r="B88" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C93, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C94, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C95, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C96, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C97, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C98, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C99, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C100, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (136.019738561583f, 209.782050977847f), new PointF(157.075490002711f, 186.775695271863f), new PointF(162.124561686466f, 189.174182783325f), new PointF(141.012117322773f, 215.415435213323f) },</v>
       </c>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
       <c r="F88" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G88" s="7" t="str">
+      <c r="G88" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H93, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H94, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H95, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H96, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H97, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H98, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H99, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H100, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (701.232680482186f, 169.09242467641f), new PointF(725.421282824328f, 146.15523430522f), new PointF(730.386826935502f, 150.363737053427f), new PointF(703.400617841122f, 176.252359661775f) },</v>
       </c>
-      <c r="H88" s="7"/>
-      <c r="I88" s="7"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
       <c r="K88" s="2"/>
       <c r="M88"/>
       <c r="Q88" s="2"/>
@@ -3601,21 +3724,21 @@
       <c r="A102" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B102" s="7" t="str">
+      <c r="B102" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C107, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C108, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C109, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C110, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C111, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C112, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C113, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C114, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (152.642670387251f, 183.239003357508f), new PointF(160.004813311712f, 159.493372269801f), new PointF(161.714293903495f, 159.475608495291f), new PointF(154.205883238813f, 183.981680313074f) },</v>
       </c>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
       <c r="F102" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G102" s="7" t="str">
+      <c r="G102" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H107, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H108, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H109, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H110, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H111, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H112, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H113, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H114, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (721.855486971315f, 141.048527086324f), new PointF(729.501472461425f, 116.638455241424f), new PointF(731.432811356851f, 116.698171759988f), new PointF(723.65227466385f, 142.57167626237f) },</v>
       </c>
-      <c r="H102" s="7"/>
-      <c r="I102" s="7"/>
+      <c r="H102" s="8"/>
+      <c r="I102" s="8"/>
       <c r="K102" s="2"/>
       <c r="M102"/>
       <c r="Q102" s="2"/>
@@ -3932,21 +4055,21 @@
       <c r="A116" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B116" s="7" t="str">
+      <c r="B116" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(C121, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C122, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C123, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C124, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C125, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C126, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(C127, ",", ".") &amp; "f, " &amp; SUBSTITUTE(C128, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (155.202544817528f, 184.45525498245f), new PointF(162.703774378685f, 159.465403773764f), new PointF(171.402358464443f, 159.37469513797f), new PointF(162.724939736444f, 188.029175232746f) },</v>
       </c>
-      <c r="C116" s="7"/>
-      <c r="D116" s="7"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
       <c r="F116" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G116" s="7" t="str">
+      <c r="G116" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp; SUBSTITUTE(H121, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H122, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H123, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H124, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H125, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H126, ",", ".") &amp; "f), new PointF(" &amp; SUBSTITUTE(H127, ",", ".") &amp; "f, " &amp; SUBSTITUTE(H128, ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (724.447298414639f, 143.245187883143f), new PointF(732.249000465397f, 116.723494587481f), new PointF(738.732781042897f, 116.924565396825f), new PointF(731.175992417625f, 148.948115406062f) },</v>
       </c>
-      <c r="H116" s="7"/>
-      <c r="I116" s="7"/>
+      <c r="H116" s="8"/>
+      <c r="I116" s="8"/>
       <c r="K116" s="2"/>
       <c r="M116"/>
       <c r="Q116" s="2"/>
@@ -4263,7 +4386,7 @@
       <c r="A130" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B130" s="7" t="str">
+      <c r="B130" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
 SUBSTITUTE(TEXT(C135, "0,00"), ",", ".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(C136, "0,00"), ",", ".") &amp; "f), new PointF(" &amp;
@@ -4275,12 +4398,12 @@
 SUBSTITUTE(TEXT(C142, "0,00"), ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (120.43f, 215.63f), new PointF(128.50f, 211.51f), new PointF(132.29f, 218.01f), new PointF(124.24f, 222.78f) },</v>
       </c>
-      <c r="C130" s="7"/>
-      <c r="D130" s="7"/>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
       <c r="F130" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G130" s="7" t="str">
+      <c r="G130" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
 SUBSTITUTE(TEXT(H135, "0,00"), ",", ".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(H136, "0,00"), ",", ".") &amp; "f), new PointF(" &amp;
@@ -4292,8 +4415,8 @@
 SUBSTITUTE(TEXT(H142, "0,00"), ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (685.45f, 173.13f), new PointF(693.84f, 170.15f), new PointF(694.65f, 177.28f), new PointF(686.09f, 180.39f) },</v>
       </c>
-      <c r="H130" s="7"/>
-      <c r="I130" s="7"/>
+      <c r="H130" s="8"/>
+      <c r="I130" s="8"/>
       <c r="K130" s="2"/>
       <c r="M130"/>
       <c r="Q130" s="2"/>
@@ -4604,9 +4727,9 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B144" s="7" t="str">
+        <v>276</v>
+      </c>
+      <c r="B144" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
 SUBSTITUTE(TEXT(C149, "0,00"), ",", ".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(C150, "0,00"), ",", ".") &amp; "f), new PointF(" &amp;
@@ -4618,12 +4741,12 @@
 SUBSTITUTE(TEXT(C156, "0,00"), ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (92.00f, 111.85f), new PointF(72.65f, 125.87f), new PointF(64.69f, 117.36f), new PointF(87.98f, 102.65f) },</v>
       </c>
-      <c r="C144" s="7"/>
-      <c r="D144" s="7"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
       <c r="F144" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="G144" s="7" t="str">
+        <v>276</v>
+      </c>
+      <c r="G144" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
 SUBSTITUTE(TEXT(H149, "0,00"), ",", ".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(H150, "0,00"), ",", ".") &amp; "f), new PointF(" &amp;
@@ -4635,8 +4758,8 @@
 SUBSTITUTE(TEXT(H156, "0,00"), ",", ".") &amp; "f) },"</f>
         <v>new PointF[4] { new PointF (655.93f, 71.53f), new PointF(640.17f, 86.63f), new PointF(629.79f, 80.02f), new PointF(649.91f, 63.27f) },</v>
       </c>
-      <c r="H144" s="7"/>
-      <c r="I144" s="7"/>
+      <c r="H144" s="8"/>
+      <c r="I144" s="8"/>
       <c r="K144" s="2"/>
       <c r="M144"/>
       <c r="Q144" s="2"/>
@@ -4646,13 +4769,13 @@
         <v>10</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="F145" t="s">
         <v>10</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="K145" s="2"/>
       <c r="M145"/>
@@ -4662,13 +4785,13 @@
         <v>11</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="F146" t="s">
         <v>11</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="K146" s="2"/>
       <c r="M146"/>
@@ -4678,13 +4801,13 @@
         <v>4</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="F147" t="s">
         <v>4</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="K147" s="2"/>
       <c r="M147"/>
@@ -4694,13 +4817,13 @@
         <v>5</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="F148" t="s">
         <v>5</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="K148" s="2"/>
       <c r="M148"/>
@@ -4710,7 +4833,7 @@
         <v>14</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C149">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B149,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4723,7 +4846,7 @@
         <v>14</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="H149">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G149,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4740,7 +4863,7 @@
         <v>15</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="C150">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B150,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4753,7 +4876,7 @@
         <v>15</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="H150">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G150,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4770,7 +4893,7 @@
         <v>16</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="C151">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B151,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4783,7 +4906,7 @@
         <v>16</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="H151">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G151,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4860,7 +4983,7 @@
         <v>19</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="C154">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B154,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4873,7 +4996,7 @@
         <v>19</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="H154">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G154,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4890,7 +5013,7 @@
         <v>20</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="C155">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B155,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4903,7 +5026,7 @@
         <v>20</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="H155">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G155,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4920,7 +5043,7 @@
         <v>21</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="C156">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B156,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4933,7 +5056,7 @@
         <v>21</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="H156">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G156,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4947,13 +5070,13 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K159" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K159" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="M159"/>
     </row>
@@ -4964,37 +5087,37 @@
       <c r="A161" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B161" s="7" t="str">
+      <c r="B161" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(C162,",",".") &amp; "f, " &amp; SUBSTITUTE(C163,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(C164,",",".") &amp; "f, " &amp; SUBSTITUTE(C165,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(C166,",",".") &amp; "f, " &amp; SUBSTITUTE(C167,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(C168,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(78.7676348023617f, 197.045802607026f), PixelSize1 = new SizeF(3.75987462459764f, 5.14884893927504f), PixelSize2 = new SizeF(6.62400107264758f, 9.12188718706622f), Degrees = 40f },</v>
       </c>
-      <c r="C161" s="7"/>
-      <c r="D161" s="7"/>
+      <c r="C161" s="8"/>
+      <c r="D161" s="8"/>
       <c r="F161" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G161" s="7" t="str">
+      <c r="G161" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(H162,",",".") &amp; "f, " &amp; SUBSTITUTE(H163,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(H164,",",".") &amp; "f, " &amp; SUBSTITUTE(H165,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(H166,",",".") &amp; "f, " &amp; SUBSTITUTE(H167,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(H168,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(645.372198995559f, 151.289343091178f), PixelSize1 = new SizeF(4.38803220663234f, 5.85486448787416f), PixelSize2 = new SizeF(6.98456806016931f, 8.64037551205804f), Degrees = 60f },</v>
       </c>
-      <c r="H161" s="7"/>
-      <c r="I161" s="7"/>
+      <c r="H161" s="8"/>
+      <c r="I161" s="8"/>
       <c r="K161" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L161" s="7" t="str">
+      <c r="L161" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(M162,",",".") &amp; "f, " &amp; SUBSTITUTE(M163,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(M164,",",".") &amp; "f, " &amp; SUBSTITUTE(M165,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(M166,",",".") &amp; "f, " &amp; SUBSTITUTE(M167,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(M168,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(262.575160629947f, 583.607457192202f), PixelSize1 = new SizeF(5.80724503487562f, 11.4602802273139f), PixelSize2 = new SizeF(6.62400107264758f, 9.12188718706622f), Degrees = 70f },</v>
       </c>
-      <c r="M161" s="7"/>
-      <c r="N161" s="7"/>
+      <c r="M161" s="8"/>
+      <c r="N161" s="8"/>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>10</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C162">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B162,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5007,7 +5130,7 @@
         <v>10</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="H162">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G162,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5035,7 +5158,7 @@
         <v>11</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C163">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B163,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5048,7 +5171,7 @@
         <v>11</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="H163">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G163,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5073,10 +5196,10 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C164">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B164,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5086,10 +5209,10 @@
         <v>6</v>
       </c>
       <c r="F164" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="H164">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G164,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5099,7 +5222,7 @@
         <v>6</v>
       </c>
       <c r="K164" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="L164" s="3" t="s">
         <v>150</v>
@@ -5114,10 +5237,10 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="C165">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B165,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5127,10 +5250,10 @@
         <v>6</v>
       </c>
       <c r="F165" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="H165">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G165,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5140,7 +5263,7 @@
         <v>6</v>
       </c>
       <c r="K165" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="L165" s="3" t="s">
         <v>151</v>
@@ -5155,10 +5278,10 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5168,10 +5291,10 @@
         <v>6</v>
       </c>
       <c r="F166" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="H166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5181,10 +5304,10 @@
         <v>6</v>
       </c>
       <c r="K166" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="L166" s="3" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="M166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5196,10 +5319,10 @@
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5209,10 +5332,10 @@
         <v>6</v>
       </c>
       <c r="F167" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="H167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5222,10 +5345,10 @@
         <v>6</v>
       </c>
       <c r="K167" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="L167" s="3" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="M167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5240,7 +5363,7 @@
         <v>141</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="C168">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B168,".",",")," deg",""))</f>
@@ -5285,37 +5408,37 @@
       <c r="A170" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B170" s="7" t="str">
+      <c r="B170" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(C171,",",".") &amp; "f, " &amp; SUBSTITUTE(C172,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(C173,",",".") &amp; "f, " &amp; SUBSTITUTE(C174,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(C175,",",".") &amp; "f, " &amp; SUBSTITUTE(C176,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(C177,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(89.3994475476303f, 168.448015409621f), PixelSize1 = new SizeF(11.1730411793682f, 10.7433040518897f), PixelSize2 = new SizeF(13.9683802147044f, 13.8644370285125f), Degrees = 60f },</v>
       </c>
-      <c r="C170" s="7"/>
-      <c r="D170" s="7"/>
+      <c r="C170" s="8"/>
+      <c r="D170" s="8"/>
       <c r="F170" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G170" s="7" t="str">
+      <c r="G170" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(H171,",",".") &amp; "f, " &amp; SUBSTITUTE(H172,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(H173,",",".") &amp; "f, " &amp; SUBSTITUTE(H174,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(H175,",",".") &amp; "f, " &amp; SUBSTITUTE(H176,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(H177,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(655.591287264545f, 125.473287391466f), PixelSize1 = new SizeF(10.0267102850775f, 9.31539894342744f), PixelSize2 = new SizeF(12.8326319992927f, 12.1194296474193f), Degrees = 62.1f },</v>
       </c>
-      <c r="H170" s="7"/>
-      <c r="I170" s="7"/>
+      <c r="H170" s="8"/>
+      <c r="I170" s="8"/>
       <c r="K170" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="L170" s="7" t="str">
+      <c r="L170" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(M171,",",".") &amp; "f, " &amp; SUBSTITUTE(M172,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(M173,",",".") &amp; "f, " &amp; SUBSTITUTE(M174,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(M175,",",".") &amp; "f, " &amp; SUBSTITUTE(M176,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(M177,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(274.061146741882f, 554.067056087834f), PixelSize1 = new SizeF(11.9108050783645f, 13.9702637702726f), PixelSize2 = new SizeF(6.62400107264758f, 9.12188718706622f), Degrees = 59.9f },</v>
       </c>
-      <c r="M170" s="7"/>
-      <c r="N170" s="7"/>
+      <c r="M170" s="8"/>
+      <c r="N170" s="8"/>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>10</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C171">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B171,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5328,7 +5451,7 @@
         <v>10</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="H171">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G171,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5356,7 +5479,7 @@
         <v>11</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C172">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B172,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5369,7 +5492,7 @@
         <v>11</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="H172">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G172,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5394,10 +5517,10 @@
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>236</v>
+      </c>
+      <c r="B173" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="C173">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B173,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5407,10 +5530,10 @@
         <v>6</v>
       </c>
       <c r="F173" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="H173">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G173,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5420,7 +5543,7 @@
         <v>6</v>
       </c>
       <c r="K173" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="L173" s="3" t="s">
         <v>144</v>
@@ -5435,10 +5558,10 @@
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>237</v>
+      </c>
+      <c r="B174" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="C174">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B174,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5448,10 +5571,10 @@
         <v>6</v>
       </c>
       <c r="F174" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="H174">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G174,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5461,7 +5584,7 @@
         <v>6</v>
       </c>
       <c r="K174" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="L174" s="3" t="s">
         <v>155</v>
@@ -5476,10 +5599,10 @@
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="C175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5489,10 +5612,10 @@
         <v>6</v>
       </c>
       <c r="F175" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5502,10 +5625,10 @@
         <v>6</v>
       </c>
       <c r="K175" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="L175" s="3" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="M175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5517,10 +5640,10 @@
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5530,10 +5653,10 @@
         <v>6</v>
       </c>
       <c r="F176" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="H176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5543,10 +5666,10 @@
         <v>6</v>
       </c>
       <c r="K176" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="L176" s="3" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="M176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5556,12 +5679,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>141</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C177">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B177,".",",")," deg",""))</f>
@@ -5597,46 +5720,46 @@
         <v>161</v>
       </c>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G178" s="3"/>
       <c r="L178" s="3"/>
       <c r="M178"/>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B179" s="7" t="str">
+      <c r="B179" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(C180,",",".") &amp; "f, " &amp; SUBSTITUTE(C181,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(C182,",",".") &amp; "f, " &amp; SUBSTITUTE(C183,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(C184,",",".") &amp; "f, " &amp; SUBSTITUTE(C185,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(C186,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(120.313342317405f, 129.814829472171f), PixelSize1 = new SizeF(7.31716653922499f, 8.84106836875298f), PixelSize2 = new SizeF(9.9715291737796f, 11.56346130053f), Degrees = 75f },</v>
       </c>
-      <c r="C179" s="7"/>
-      <c r="D179" s="7"/>
+      <c r="C179" s="8"/>
+      <c r="D179" s="8"/>
       <c r="F179" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G179" s="7" t="str">
+      <c r="G179" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(H180,",",".") &amp; "f, " &amp; SUBSTITUTE(H181,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(H182,",",".") &amp; "f, " &amp; SUBSTITUTE(H183,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(H184,",",".") &amp; "f, " &amp; SUBSTITUTE(H185,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(H186,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(683.08659880357f, 85.4726687694167f), PixelSize1 = new SizeF(8.2223635362004f, 10.2194616801775f), PixelSize2 = new SizeF(10.3714032542806f, 12.3594295796251f), Degrees = 80f },</v>
       </c>
-      <c r="H179" s="7"/>
-      <c r="I179" s="7"/>
+      <c r="H179" s="8"/>
+      <c r="I179" s="8"/>
       <c r="K179" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="L179" s="7" t="str">
+      <c r="L179" s="8" t="str">
         <f>"new Light.Spot { PixelCenter = new PointF(" &amp; SUBSTITUTE(M180,",",".") &amp; "f, " &amp; SUBSTITUTE(M181,",",".") &amp; "f), PixelSize1 = new SizeF(" &amp; SUBSTITUTE(M182,",",".") &amp; "f, " &amp; SUBSTITUTE(M183,",",".") &amp; "f), PixelSize2 = new SizeF(" &amp; SUBSTITUTE(M184,",",".") &amp; "f, " &amp; SUBSTITUTE(M185,",",".") &amp; "f), Degrees = " &amp; SUBSTITUTE(M186,",",".") &amp; "f },"</f>
         <v>new Light.Spot { PixelCenter = new PointF(303.938694887144f, 517.110846054632f), PixelSize1 = new SizeF(7.20302478845816f, 12.9161538318128f), PixelSize2 = new SizeF(6.62400107264758f, 9.12188718706622f), Degrees = 70f },</v>
       </c>
-      <c r="M179" s="7"/>
-      <c r="N179" s="7"/>
-    </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M179" s="8"/>
+      <c r="N179" s="8"/>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>10</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C180">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B180,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5649,7 +5772,7 @@
         <v>10</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="H180">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G180,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5672,12 +5795,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>11</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C181">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B181,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5690,7 +5813,7 @@
         <v>11</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="H181">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G181,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5713,12 +5836,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C182">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B182,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5728,10 +5851,10 @@
         <v>6</v>
       </c>
       <c r="F182" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="H182">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G182,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5741,7 +5864,7 @@
         <v>6</v>
       </c>
       <c r="K182" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="L182" s="3" t="s">
         <v>159</v>
@@ -5754,12 +5877,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="C183">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B183,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5769,10 +5892,10 @@
         <v>6</v>
       </c>
       <c r="F183" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="H183">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G183,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5795,12 +5918,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5810,10 +5933,10 @@
         <v>6</v>
       </c>
       <c r="F184" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="H184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5823,10 +5946,10 @@
         <v>6</v>
       </c>
       <c r="K184" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="L184" s="3" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="M184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5836,12 +5959,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="C185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5851,10 +5974,10 @@
         <v>6</v>
       </c>
       <c r="F185" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="H185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5864,10 +5987,10 @@
         <v>6</v>
       </c>
       <c r="K185" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="L185" s="3" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="M185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5877,7 +6000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>141</v>
       </c>
@@ -5918,994 +6041,789 @@
         <v>161</v>
       </c>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K187" s="2"/>
       <c r="M187"/>
     </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>10</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H189" s="7" t="str">
+        <f>"new Number { Target = """ &amp; A188 &amp; """, PixelCenter = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B189,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B190,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), PixelSize = new SizeF("&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B191,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B192,".",",")," mm",""))*$B$3/$B$7, "0,00"),",",".")&amp;"f), Degrees = "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B193,".",",")," deg","")), "0,00"),",",".")&amp;"f, OrientStart = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B196,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B197,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B194,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B195,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
+        <v>new Number { Target = "Ball 1", PixelCenter = new PointF(124.72f, 175.53f), PixelSize = new SizeF(90.68f, 95.44f), Degrees = -24.00f, OrientStart = new PointF(127.38f, 201.46f), OrientEnd = new PointF(138.72f, 156.11f) },</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>11</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H190" s="7" t="str">
+        <f>"new Number { Target = """ &amp; A199 &amp; """, PixelCenter = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B200,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B201,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), PixelSize = new SizeF("&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B202,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B203,".",",")," mm",""))*$B$3/$B$7, "0,00"),",",".")&amp;"f), Degrees = "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B204,".",",")," deg","")), "0,00"),",",".")&amp;"f, OrientStart = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B207,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B208,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B205,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B206,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
+        <v>new Number { Target = "Ball 4a", PixelCenter = new PointF(641.06f, 154.74f), PixelSize = new SizeF(74.17f, 93.62f), Degrees = 41.30f, OrientStart = new PointF(653.94f, 144.58f), OrientEnd = new PointF(644.95f, 184.83f) },</v>
+      </c>
+      <c r="K190" s="2"/>
+      <c r="M190"/>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>4</v>
+      </c>
+      <c r="B191" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F188" s="1" t="s">
+      <c r="H191" s="7" t="str">
+        <f>"new Number { Target = """ &amp; D199 &amp; """, PixelCenter = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E200,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E201,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), PixelSize = new SizeF("&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E202,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E203,".",",")," mm",""))*$B$3/$B$7, "0,00"),",",".")&amp;"f), Degrees = "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E204,".",",")," deg","")), "0,00"),",",".")&amp;"f, OrientStart = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E207,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E208,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E205,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E206,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
+        <v>new Number { Target = "Ball 4b", PixelCenter = new PointF(669.97f, 139.25f), PixelSize = new SizeF(74.17f, 93.62f), Degrees = 41.30f, OrientStart = new PointF(653.94f, 144.58f), OrientEnd = new PointF(644.95f, 184.83f) },</v>
+      </c>
+      <c r="K191" s="2"/>
+      <c r="M191"/>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>5</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H192" s="7" t="str">
+        <f>"new Number { Target = """ &amp; A210 &amp; """, PixelCenter = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B211,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B212,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), PixelSize = new SizeF("&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B213,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B214,".",",")," mm",""))*$B$3/$B$7, "0,00"),",",".")&amp;"f), Degrees = "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B215,".",",")," deg","")), "0,00"),",",".")&amp;"f, OrientStart = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B218,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B219,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B216,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B217,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
+        <v>new Number { Target = "Ball 8a", PixelCenter = new PointF(520.97f, 181.08f), PixelSize = new SizeF(98.21f, 93.10f), Degrees = 96.00f, OrientStart = new PointF(534.89f, 163.29f), OrientEnd = new PointF(510.13f, 199.19f) },</v>
+      </c>
+      <c r="K192" s="2"/>
+      <c r="M192"/>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>141</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H193" s="7" t="str">
+        <f>"new Number { Target = """ &amp; D210 &amp; """, PixelCenter = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E211,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E212,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), PixelSize = new SizeF("&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E213,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E214,".",",")," mm",""))*$B$3/$B$7, "0,00"),",",".")&amp;"f), Degrees = "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E215,".",",")," deg","")), "0,00"),",",".")&amp;"f, OrientStart = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E218,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E219,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E216,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E217,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
+        <v>new Number { Target = "Ball 8b", PixelCenter = new PointF(486.89f, 205.26f), PixelSize = new SizeF(92.53f, 94.44f), Degrees = -4.80f, OrientStart = new PointF(682.86f, 189.74f), OrientEnd = new PointF(673.86f, 169.34f) },</v>
+      </c>
+      <c r="K193" s="2"/>
+      <c r="M193"/>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>190</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H194" s="7" t="str">
+        <f>"new Number { Target = """ &amp; A221 &amp; """, PixelCenter = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B222,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B223,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), PixelSize = new SizeF("&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B224,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B225,".",",")," mm",""))*$B$3/$B$7, "0,00"),",",".")&amp;"f), Degrees = "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B226,".",",")," deg","")), "0,00"),",",".")&amp;"f, OrientStart = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B229,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B230,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B227,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B228,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
+        <v>new Number { Target = "Ball 9a", PixelCenter = new PointF(288.97f, 209.33f), PixelSize = new SizeF(90.71f, 57.60f), Degrees = 41.00f, OrientStart = new PointF(282.61f, 189.37f), OrientEnd = new PointF(302.26f, 220.74f) },</v>
+      </c>
+      <c r="K194" s="2"/>
+      <c r="M194"/>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>191</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H195" s="7" t="str">
+        <f>"new Number { Target = """ &amp; D221 &amp; """, PixelCenter = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E222,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E223,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), PixelSize = new SizeF("&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E224,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E225,".",",")," mm",""))*$B$3/$B$7, "0,00"),",",".")&amp;"f), Degrees = "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E226,".",",")," deg","")), "0,00"),",",".")&amp;"f, OrientStart = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E229,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E230,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E227,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E228,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
+        <v>new Number { Target = "Ball 9b", PixelCenter = new PointF(324.39f, 264.20f), PixelSize = new SizeF(90.71f, 90.71f), Degrees = 30.00f, OrientStart = new PointF(320.21f, 224.52f), OrientEnd = new PointF(340.53f, 259.95f) },</v>
+      </c>
+      <c r="K195" s="2"/>
+      <c r="M195"/>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>192</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H196" s="7" t="str">
+        <f>"new Number { Target = """ &amp; G221 &amp; """, PixelCenter = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(H222,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(H223,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), PixelSize = new SizeF("&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H224,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H225,".",",")," mm",""))*$B$3/$B$7, "0,00"),",",".")&amp;"f), Degrees = "&amp;
+SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H226,".",",")," deg","")), "0,00"),",",".")&amp;"f, OrientStart = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(H229,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(H230,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
+SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(H227,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
+SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(H228,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
+        <v>new Number { Target = "Ball 9c", PixelCenter = new PointF(332.01f, 279.48f), PixelSize = new SizeF(90.71f, 90.71f), Degrees = 41.00f, OrientStart = new PointF(334.29f, 262.78f), OrientEnd = new PointF(324.94f, 302.00f) },</v>
+      </c>
+      <c r="K196" s="2"/>
+      <c r="M196"/>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>193</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="K197" s="2"/>
+      <c r="M197"/>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K198" s="2"/>
+      <c r="M198"/>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B199"/>
+      <c r="D199" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="I199" s="2"/>
+      <c r="M199"/>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>10</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D200" t="s">
+        <v>10</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="I200" s="2"/>
+      <c r="M200"/>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>11</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D201" t="s">
+        <v>11</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="I201" s="2"/>
+      <c r="M201"/>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>4</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D202" t="s">
+        <v>4</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I202" s="2"/>
+      <c r="M202"/>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>5</v>
+      </c>
+      <c r="B203" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="K188" s="1" t="s">
+      <c r="D203" t="s">
+        <v>5</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F203" s="5"/>
+      <c r="I203" s="2"/>
+      <c r="M203"/>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>141</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D204" t="s">
+        <v>141</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I204" s="2"/>
+      <c r="M204"/>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>190</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D205" t="s">
+        <v>190</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I205" s="2"/>
+      <c r="M205"/>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>191</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D206" t="s">
+        <v>191</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I206" s="2"/>
+      <c r="M206"/>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>192</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D207" t="s">
+        <v>192</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I207" s="2"/>
+      <c r="M207"/>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>193</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D208" t="s">
+        <v>193</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I208" s="2"/>
+      <c r="M208"/>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I209" s="2"/>
+      <c r="M209"/>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B210"/>
+      <c r="D210" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I210" s="2"/>
+      <c r="M210"/>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>10</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D211" t="s">
+        <v>10</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H211" s="5"/>
+      <c r="I211" s="2"/>
+      <c r="M211"/>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>11</v>
+      </c>
+      <c r="B212" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="M188"/>
-      <c r="P188" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="M189"/>
-    </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B190" s="7" t="str">
-        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(C191,",",".")&amp;"f, "&amp;SUBSTITUTE(C192,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(C193,",",".")&amp;"f, "&amp;SUBSTITUTE(C194,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(C195,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(C196,",",".")&amp;"f, "&amp;SUBSTITUTE(C197,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(C198,",",".")&amp;"f, "&amp;SUBSTITUTE(C199,",",".")&amp;"f) },"</f>
-        <v>new Number { PixelCenter = new PointF(124.723673740246f, 175.531981912508f), PixelSize = new SizeF(90.681085550446f, 95.4390911509929f), Degrees = -24f, OrientStart = new PointF(138.7196445106f, 156.106349604506f), OrientEnd = new PointF(127.381059997338f, 201.460667501665f) },</v>
-      </c>
-      <c r="C190" s="7"/>
-      <c r="D190" s="7"/>
-      <c r="F190" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G190" s="7" t="str">
-        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(H191,",",".")&amp;"f, "&amp;SUBSTITUTE(H192,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(H193,",",".")&amp;"f, "&amp;SUBSTITUTE(H194,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(H195,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(H196,",",".")&amp;"f, "&amp;SUBSTITUTE(H197,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(H198,",",".")&amp;"f, "&amp;SUBSTITUTE(H199,",",".")&amp;"f) },"</f>
-        <v>new Number { PixelCenter = new PointF(641.059001446714f, 154.743074399047f), PixelSize = new SizeF(74.1679490181485f, 93.615469618878f), Degrees = 41.3f, OrientStart = new PointF(644.949647746031f, 184.830750939373f), OrientEnd = new PointF(653.944924793219f, 144.578793805644f) },</v>
-      </c>
-      <c r="H190" s="7"/>
-      <c r="I190" s="7"/>
-      <c r="K190" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="L190" s="7" t="str">
-        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(M191,",",".")&amp;"f, "&amp;SUBSTITUTE(M192,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(M193,",",".")&amp;"f, "&amp;SUBSTITUTE(M194,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(M195,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(M196,",",".")&amp;"f, "&amp;SUBSTITUTE(M197,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(M198,",",".")&amp;"f, "&amp;SUBSTITUTE(M199,",",".")&amp;"f) },"</f>
-        <v>new Number { PixelCenter = new PointF(520.968651291404f, 181.078059086033f), PixelSize = new SizeF(98.2144411010572f, 93.1022099213418f), Degrees = 96f, OrientStart = new PointF(510.133877883348f, 199.192951606807f), OrientEnd = new PointF(534.889787403969f, 163.287449938223f) },</v>
-      </c>
-      <c r="M190" s="7"/>
-      <c r="N190" s="7"/>
-      <c r="P190" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q190" s="7" t="str">
-        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(R191,",",".")&amp;"f, "&amp;SUBSTITUTE(R192,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(R193,",",".")&amp;"f, "&amp;SUBSTITUTE(R194,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(R195,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(R196,",",".")&amp;"f, "&amp;SUBSTITUTE(R197,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(R198,",",".")&amp;"f, "&amp;SUBSTITUTE(R199,",",".")&amp;"f) },"</f>
-        <v>new Number { PixelCenter = new PointF(486.888267819892f, 205.256068004359f), PixelSize = new SizeF(92.5296527789248f, 94.4443197784486f), Degrees = -4.8f, OrientStart = new PointF(473.283478215247f, 225.271684397674f), OrientEnd = new PointF(498.228364144423f, 189.744135378232f) },</v>
-      </c>
-      <c r="R190" s="7"/>
-      <c r="S190" s="7"/>
-    </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="D212" t="s">
+        <v>11</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H212" s="5"/>
+      <c r="I212" s="2"/>
+      <c r="M212"/>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>4</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D213" t="s">
+        <v>4</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H213" s="5"/>
+      <c r="I213" s="2"/>
+      <c r="M213"/>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>5</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D214" t="s">
+        <v>5</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="H214" s="5"/>
+      <c r="I214" s="2"/>
+      <c r="M214"/>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>141</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D215" t="s">
+        <v>141</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="H215" s="5"/>
+      <c r="I215" s="2"/>
+      <c r="M215"/>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>190</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D216" t="s">
+        <v>190</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="F216" s="5"/>
+      <c r="H216" s="5"/>
+      <c r="I216" s="2"/>
+      <c r="M216"/>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>191</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D217" t="s">
+        <v>191</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="H217" s="5"/>
+      <c r="I217" s="2"/>
+      <c r="M217"/>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>192</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D218" t="s">
+        <v>192</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="H218" s="5"/>
+      <c r="I218" s="2"/>
+      <c r="M218"/>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>193</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D219" t="s">
+        <v>193</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H219" s="5"/>
+      <c r="I219" s="2"/>
+      <c r="M219"/>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H220" s="5"/>
+      <c r="I220" s="2"/>
+      <c r="M220"/>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B221"/>
+      <c r="D221" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G221" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H221" s="5"/>
+      <c r="I221" s="2"/>
+      <c r="M221"/>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>10</v>
       </c>
-      <c r="B191" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C191">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B191,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>124.72367374024631</v>
-      </c>
-      <c r="D191" t="s">
-        <v>6</v>
-      </c>
-      <c r="F191" t="s">
+      <c r="B222" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D222" t="s">
         <v>10</v>
       </c>
-      <c r="G191" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H191">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G191,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>641.05900144671398</v>
-      </c>
-      <c r="I191" t="s">
-        <v>6</v>
-      </c>
-      <c r="K191" t="s">
+      <c r="E222" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G222" t="s">
         <v>10</v>
       </c>
-      <c r="L191" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="M191">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L191,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>520.9686512914036</v>
-      </c>
-      <c r="N191" t="s">
-        <v>6</v>
-      </c>
-      <c r="P191" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q191" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="R191">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(Q191,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>486.88826781989235</v>
-      </c>
-      <c r="S191" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="H222" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="I222" s="2"/>
+      <c r="M222"/>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>11</v>
       </c>
-      <c r="B192" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C192">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B192,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>175.53198191250829</v>
-      </c>
-      <c r="D192" t="s">
-        <v>6</v>
-      </c>
-      <c r="F192" t="s">
+      <c r="B223" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D223" t="s">
         <v>11</v>
       </c>
-      <c r="G192" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="H192">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G192,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>154.7430743990468</v>
-      </c>
-      <c r="I192" t="s">
-        <v>6</v>
-      </c>
-      <c r="K192" t="s">
+      <c r="E223" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G223" t="s">
         <v>11</v>
       </c>
-      <c r="L192" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="M192">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L192,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>181.07805908603262</v>
-      </c>
-      <c r="N192" t="s">
-        <v>6</v>
-      </c>
-      <c r="P192" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q192" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="R192">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(Q192,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>205.25606800435924</v>
-      </c>
-      <c r="S192" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="H223" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="I223" s="2"/>
+      <c r="M223"/>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>4</v>
       </c>
-      <c r="B193" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C193">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B193,".",",")," mm",""))*$B$2/$B$6</f>
-        <v>90.681085550446014</v>
-      </c>
-      <c r="D193" t="s">
-        <v>6</v>
-      </c>
-      <c r="F193" t="s">
+      <c r="B224" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D224" t="s">
         <v>4</v>
       </c>
-      <c r="G193" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H193">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G193,".",",")," mm",""))*$B$2/$B$6</f>
-        <v>74.167949018148533</v>
-      </c>
-      <c r="I193" t="s">
-        <v>6</v>
-      </c>
-      <c r="K193" t="s">
+      <c r="E224" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="G224" t="s">
         <v>4</v>
       </c>
-      <c r="L193" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="M193">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L193,".",",")," mm",""))*$B$2/$B$6</f>
-        <v>98.214441101057204</v>
-      </c>
-      <c r="N193" t="s">
-        <v>6</v>
-      </c>
-      <c r="P193" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q193" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="R193">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(Q193,".",",")," mm",""))*$B$2/$B$6</f>
-        <v>92.529652778924813</v>
-      </c>
-      <c r="S193" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="H224" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="I224" s="2"/>
+      <c r="M224"/>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>5</v>
       </c>
-      <c r="B194" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C194">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B194,".",",")," mm",""))*$B$3/$B$7</f>
-        <v>95.439091150992923</v>
-      </c>
-      <c r="D194" t="s">
-        <v>6</v>
-      </c>
-      <c r="F194" t="s">
+      <c r="B225" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D225" t="s">
         <v>5</v>
       </c>
-      <c r="G194" s="3" t="s">
+      <c r="E225" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="G225" t="s">
+        <v>5</v>
+      </c>
+      <c r="H225" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="I225" s="2"/>
+      <c r="M225"/>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>141</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D226" t="s">
+        <v>141</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G226" t="s">
+        <v>141</v>
+      </c>
+      <c r="H226" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="I226" s="2"/>
+      <c r="M226"/>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>190</v>
       </c>
-      <c r="H194">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G194,".",",")," mm",""))*$B$3/$B$7</f>
-        <v>93.615469618877967</v>
-      </c>
-      <c r="I194" t="s">
-        <v>6</v>
-      </c>
-      <c r="K194" t="s">
-        <v>5</v>
-      </c>
-      <c r="L194" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="M194">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L194,".",",")," mm",""))*$B$3/$B$7</f>
-        <v>93.102209921341782</v>
-      </c>
-      <c r="N194" t="s">
-        <v>6</v>
-      </c>
-      <c r="P194" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q194" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="R194">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(Q194,".",",")," mm",""))*$B$3/$B$7</f>
-        <v>94.444319778448559</v>
-      </c>
-      <c r="S194" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>141</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C195">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B195,".",",")," deg",""))</f>
-        <v>-24</v>
-      </c>
-      <c r="D195" t="s">
-        <v>161</v>
-      </c>
-      <c r="F195" t="s">
-        <v>141</v>
-      </c>
-      <c r="G195" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H195">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G195,".",",")," deg",""))</f>
-        <v>41.3</v>
-      </c>
-      <c r="I195" t="s">
-        <v>161</v>
-      </c>
-      <c r="K195" t="s">
-        <v>141</v>
-      </c>
-      <c r="L195" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="M195">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L195,".",",")," deg",""))</f>
-        <v>96</v>
-      </c>
-      <c r="N195" t="s">
-        <v>161</v>
-      </c>
-      <c r="P195" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q195" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="R195">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(Q195,".",",")," deg",""))</f>
-        <v>-4.8</v>
-      </c>
-      <c r="S195" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>195</v>
-      </c>
-      <c r="B196" s="3" t="s">
+      <c r="B227" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D227" t="s">
+        <v>190</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="G227" t="s">
+        <v>190</v>
+      </c>
+      <c r="H227" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="M227"/>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>191</v>
       </c>
-      <c r="C196">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B196,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>138.71964451059966</v>
-      </c>
-      <c r="D196" t="s">
-        <v>6</v>
-      </c>
-      <c r="F196" t="s">
-        <v>195</v>
-      </c>
-      <c r="G196" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H196">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G196,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>644.94964774603125</v>
-      </c>
-      <c r="I196" t="s">
-        <v>6</v>
-      </c>
-      <c r="K196" t="s">
-        <v>195</v>
-      </c>
-      <c r="L196" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="M196">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L196,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>510.13387788334762</v>
-      </c>
-      <c r="N196" t="s">
-        <v>6</v>
-      </c>
-      <c r="P196" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q196" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="R196">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(Q196,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>473.28347821524653</v>
-      </c>
-      <c r="S196" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>196</v>
-      </c>
-      <c r="B197" s="3" t="s">
+      <c r="B228" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D228" t="s">
+        <v>191</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G228" t="s">
+        <v>191</v>
+      </c>
+      <c r="H228" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="M228"/>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
         <v>192</v>
       </c>
-      <c r="C197">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B197,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>156.10634960450568</v>
-      </c>
-      <c r="D197" t="s">
-        <v>6</v>
-      </c>
-      <c r="F197" t="s">
-        <v>196</v>
-      </c>
-      <c r="G197" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H197">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G197,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>184.83075093937339</v>
-      </c>
-      <c r="I197" t="s">
-        <v>6</v>
-      </c>
-      <c r="K197" t="s">
-        <v>196</v>
-      </c>
-      <c r="L197" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="M197">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L197,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>199.1929516068073</v>
-      </c>
-      <c r="N197" t="s">
-        <v>6</v>
-      </c>
-      <c r="P197" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q197" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="R197">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(Q197,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>225.27168439767394</v>
-      </c>
-      <c r="S197" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>197</v>
-      </c>
-      <c r="B198" s="3" t="s">
+      <c r="B229" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D229" t="s">
+        <v>192</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="F229" s="5"/>
+      <c r="G229" t="s">
+        <v>192</v>
+      </c>
+      <c r="H229" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="I229" s="5"/>
+      <c r="J229" s="5"/>
+      <c r="M229"/>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>193</v>
       </c>
-      <c r="C198">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B198,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>127.38105999733779</v>
-      </c>
-      <c r="D198" t="s">
-        <v>6</v>
-      </c>
-      <c r="F198" t="s">
-        <v>197</v>
-      </c>
-      <c r="G198" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H198">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G198,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>653.944924793219</v>
-      </c>
-      <c r="I198" t="s">
-        <v>6</v>
-      </c>
-      <c r="K198" t="s">
-        <v>197</v>
-      </c>
-      <c r="L198" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="M198">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L198,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>534.88978740396942</v>
-      </c>
-      <c r="N198" t="s">
-        <v>6</v>
-      </c>
-      <c r="P198" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q198" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="R198">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(Q198,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>498.2283641444227</v>
-      </c>
-      <c r="S198" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>198</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C199">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B199,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>201.46066750166523</v>
-      </c>
-      <c r="D199" t="s">
-        <v>6</v>
-      </c>
-      <c r="F199" t="s">
-        <v>198</v>
-      </c>
-      <c r="G199" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="H199">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G199,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>144.57879380564418</v>
-      </c>
-      <c r="I199" t="s">
-        <v>6</v>
-      </c>
-      <c r="K199" t="s">
-        <v>198</v>
-      </c>
-      <c r="L199" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="M199">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L199,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>163.28744993822261</v>
-      </c>
-      <c r="N199" t="s">
-        <v>6</v>
-      </c>
-      <c r="P199" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q199" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="R199">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(Q199,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>189.74413537823239</v>
-      </c>
-      <c r="S199" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B201"/>
-      <c r="F201" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="K201" s="1" t="s">
+      <c r="B230" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D230" t="s">
+        <v>193</v>
+      </c>
+      <c r="E230" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="M201"/>
-    </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B202"/>
-      <c r="M202"/>
-    </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B203" s="7" t="str">
-        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(C204,",",".")&amp;"f, "&amp;SUBSTITUTE(C205,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(C206,",",".")&amp;"f, "&amp;SUBSTITUTE(C207,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(C208,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(C209,",",".")&amp;"f, "&amp;SUBSTITUTE(C210,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(C211,",",".")&amp;"f, "&amp;SUBSTITUTE(C212,",",".")&amp;"f) },"</f>
-        <v>new Number { PixelCenter = new PointF(288.97025151837f, 209.327373940928f), PixelSize = new SizeF(90.708676106095f, 57.5992278240944f), Degrees = 41f, OrientStart = new PointF(302.259828473547f, 220.736252607958f), OrientEnd = new PointF(282.606281983893f, 189.366182729089f) },</v>
-      </c>
-      <c r="C203" s="7"/>
-      <c r="D203" s="7"/>
-      <c r="F203" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G203" s="7" t="str">
-        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(H204,",",".")&amp;"f, "&amp;SUBSTITUTE(H205,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(H206,",",".")&amp;"f, "&amp;SUBSTITUTE(H207,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(H208,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(H209,",",".")&amp;"f, "&amp;SUBSTITUTE(H210,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(H211,",",".")&amp;"f, "&amp;SUBSTITUTE(H212,",",".")&amp;"f) },"</f>
-        <v>new Number { PixelCenter = new PointF(324.389721820897f, 264.19778363821f), PixelSize = new SizeF(90.708676106095f, 90.7086357943192f), Degrees = 30f, OrientStart = new PointF(340.527551205805f, 259.948839956544f), OrientEnd = new PointF(320.212587286211f, 224.515779099388f) },</v>
-      </c>
-      <c r="H203" s="7"/>
-      <c r="I203" s="7"/>
-      <c r="K203" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="L203" s="7" t="str">
-        <f>"new Number { PixelCenter = new PointF("&amp;SUBSTITUTE(M204,",",".")&amp;"f, "&amp;SUBSTITUTE(M205,",",".")&amp;"f), PixelSize = new SizeF("&amp;SUBSTITUTE(M206,",",".")&amp;"f, "&amp;SUBSTITUTE(M207,",",".")&amp;"f), Degrees = "&amp;SUBSTITUTE(M208,",",".")&amp;"f, OrientStart = new PointF("&amp;SUBSTITUTE(M209,",",".")&amp;"f, "&amp;SUBSTITUTE(M210,",",".")&amp;"f), OrientEnd = new PointF("&amp;SUBSTITUTE(M211,",",".")&amp;"f, "&amp;SUBSTITUTE(M212,",",".")&amp;"f) },"</f>
-        <v>new Number { PixelCenter = new PointF(332.014164000431f, 279.4833226275f), PixelSize = new SizeF(90.708676106095f, 90.7086357943192f), Degrees = 41f, OrientStart = new PointF(324.93699750007f, 301.996072173702f), OrientEnd = new PointF(334.291329723511f, 262.783484825116f) },</v>
-      </c>
-      <c r="M203" s="7"/>
-      <c r="N203" s="7"/>
-    </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>10</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="C204">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B204,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>288.97025151836959</v>
-      </c>
-      <c r="D204" t="s">
-        <v>6</v>
-      </c>
-      <c r="F204" t="s">
-        <v>10</v>
-      </c>
-      <c r="G204" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="H204">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G204,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>324.38972182089697</v>
-      </c>
-      <c r="I204" t="s">
-        <v>6</v>
-      </c>
-      <c r="K204" t="s">
-        <v>10</v>
-      </c>
-      <c r="L204" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="M204">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L204,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>332.01416400043138</v>
-      </c>
-      <c r="N204" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>11</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="C205">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B205,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>209.3273739409276</v>
-      </c>
-      <c r="D205" t="s">
-        <v>6</v>
-      </c>
-      <c r="F205" t="s">
-        <v>11</v>
-      </c>
-      <c r="G205" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="H205">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G205,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>264.1977836382095</v>
-      </c>
-      <c r="I205" t="s">
-        <v>6</v>
-      </c>
-      <c r="K205" t="s">
-        <v>11</v>
-      </c>
-      <c r="L205" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="M205">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L205,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>279.48332262749966</v>
-      </c>
-      <c r="N205" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>4</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="C206">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B206,".",",")," mm",""))*$B$2/$B$6</f>
-        <v>90.708676106094956</v>
-      </c>
-      <c r="D206" t="s">
-        <v>6</v>
-      </c>
-      <c r="F206" t="s">
-        <v>4</v>
-      </c>
-      <c r="G206" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="H206">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G206,".",",")," mm",""))*$B$2/$B$6</f>
-        <v>90.708676106094956</v>
-      </c>
-      <c r="I206" t="s">
-        <v>6</v>
-      </c>
-      <c r="K206" t="s">
-        <v>4</v>
-      </c>
-      <c r="L206" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="M206">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L206,".",",")," mm",""))*$B$2/$B$6</f>
-        <v>90.708676106094956</v>
-      </c>
-      <c r="N206" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>5</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="C207">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B207,".",",")," mm",""))*$B$3/$B$7</f>
-        <v>57.599227824094392</v>
-      </c>
-      <c r="D207" t="s">
-        <v>6</v>
-      </c>
-      <c r="F207" t="s">
-        <v>5</v>
-      </c>
-      <c r="G207" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="H207">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G207,".",",")," mm",""))*$B$3/$B$7</f>
-        <v>90.708635794319179</v>
-      </c>
-      <c r="I207" t="s">
-        <v>6</v>
-      </c>
-      <c r="K207" t="s">
-        <v>5</v>
-      </c>
-      <c r="L207" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="M207">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L207,".",",")," mm",""))*$B$3/$B$7</f>
-        <v>90.708635794319179</v>
-      </c>
-      <c r="N207" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>141</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="C208">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B208,".",",")," deg",""))</f>
-        <v>41</v>
-      </c>
-      <c r="D208" t="s">
-        <v>161</v>
-      </c>
-      <c r="F208" t="s">
-        <v>141</v>
-      </c>
-      <c r="G208" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="H208">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G208,".",",")," deg",""))</f>
-        <v>30</v>
-      </c>
-      <c r="I208" t="s">
-        <v>161</v>
-      </c>
-      <c r="K208" t="s">
-        <v>141</v>
-      </c>
-      <c r="L208" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="M208">
-        <f>VALUE(SUBSTITUTE(SUBSTITUTE(L208,".",",")," deg",""))</f>
-        <v>41</v>
-      </c>
-      <c r="N208" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>195</v>
-      </c>
-      <c r="B209" s="3" t="s">
+      <c r="G230" t="s">
+        <v>193</v>
+      </c>
+      <c r="H230" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="C209">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B209,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>302.25982847354669</v>
-      </c>
-      <c r="D209" t="s">
-        <v>6</v>
-      </c>
-      <c r="F209" t="s">
-        <v>195</v>
-      </c>
-      <c r="G209" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H209">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G209,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>340.52755120580548</v>
-      </c>
-      <c r="I209" t="s">
-        <v>6</v>
-      </c>
-      <c r="K209" t="s">
-        <v>195</v>
-      </c>
-      <c r="L209" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="M209">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L209,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>324.93699750007039</v>
-      </c>
-      <c r="N209" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>196</v>
-      </c>
-      <c r="B210" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="C210">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B210,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>220.73625260795802</v>
-      </c>
-      <c r="D210" t="s">
-        <v>6</v>
-      </c>
-      <c r="F210" t="s">
-        <v>196</v>
-      </c>
-      <c r="G210" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="H210">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G210,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>259.94883995654396</v>
-      </c>
-      <c r="I210" t="s">
-        <v>6</v>
-      </c>
-      <c r="K210" t="s">
-        <v>196</v>
-      </c>
-      <c r="L210" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="M210">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L210,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>301.99607217370232</v>
-      </c>
-      <c r="N210" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>197</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="C211">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B211,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>282.60628198389276</v>
-      </c>
-      <c r="D211" t="s">
-        <v>6</v>
-      </c>
-      <c r="F211" t="s">
-        <v>197</v>
-      </c>
-      <c r="G211" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="H211">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G211,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>320.21258728621132</v>
-      </c>
-      <c r="I211" t="s">
-        <v>6</v>
-      </c>
-      <c r="K211" t="s">
-        <v>197</v>
-      </c>
-      <c r="L211" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="M211">
-        <f>(VALUE(SUBSTITUTE(SUBSTITUTE(L211,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
-        <v>334.29132972351147</v>
-      </c>
-      <c r="N211" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>198</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="C212">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B212,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>189.36618272908925</v>
-      </c>
-      <c r="D212" t="s">
-        <v>6</v>
-      </c>
-      <c r="F212" t="s">
-        <v>198</v>
-      </c>
-      <c r="G212" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="H212">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G212,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>224.515779099388</v>
-      </c>
-      <c r="I212" t="s">
-        <v>6</v>
-      </c>
-      <c r="K212" t="s">
-        <v>198</v>
-      </c>
-      <c r="L212" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="M212">
-        <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(L212,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
-        <v>262.78348482511643</v>
-      </c>
-      <c r="N212" t="s">
-        <v>6</v>
-      </c>
+      <c r="M230"/>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M231"/>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M232"/>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M233"/>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M234"/>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M235"/>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M236"/>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M237"/>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M238"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="B203:D203"/>
-    <mergeCell ref="G203:I203"/>
-    <mergeCell ref="L203:N203"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="B179:D179"/>
-    <mergeCell ref="G161:I161"/>
-    <mergeCell ref="G170:I170"/>
-    <mergeCell ref="G179:I179"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F23:H23"/>
+  <mergeCells count="34">
+    <mergeCell ref="B144:D144"/>
+    <mergeCell ref="G144:I144"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="G130:I130"/>
+    <mergeCell ref="L161:N161"/>
+    <mergeCell ref="L170:N170"/>
+    <mergeCell ref="L179:N179"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="G88:I88"/>
+    <mergeCell ref="G74:I74"/>
     <mergeCell ref="B116:D116"/>
     <mergeCell ref="G116:I116"/>
     <mergeCell ref="G102:I102"/>
@@ -6914,22 +6832,22 @@
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="G46:I46"/>
     <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B144:D144"/>
-    <mergeCell ref="G144:I144"/>
-    <mergeCell ref="L190:N190"/>
-    <mergeCell ref="Q190:S190"/>
-    <mergeCell ref="B190:D190"/>
-    <mergeCell ref="G190:I190"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="G130:I130"/>
-    <mergeCell ref="L161:N161"/>
-    <mergeCell ref="L170:N170"/>
-    <mergeCell ref="L179:N179"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="G88:I88"/>
-    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="B179:D179"/>
+    <mergeCell ref="G161:I161"/>
+    <mergeCell ref="G170:I170"/>
+    <mergeCell ref="G179:I179"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
- Refactoring, separated the Raytracer from Form1 - Added cloth texture - Added keyframe-animation for motion blur
</commit_message>
<xml_diff>
--- a/Documentation/Original.xlsx
+++ b/Documentation/Original.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="384">
   <si>
     <t>Pixelwidth</t>
   </si>
@@ -569,21 +569,6 @@
     <t>-24.0000 deg</t>
   </si>
   <si>
-    <t>19.6236 mm</t>
-  </si>
-  <si>
-    <t>41.3000 deg</t>
-  </si>
-  <si>
-    <t>171.8906 mm</t>
-  </si>
-  <si>
-    <t>195.9607 mm</t>
-  </si>
-  <si>
-    <t>24.7691 mm</t>
-  </si>
-  <si>
     <t>38,98 mm</t>
   </si>
   <si>
@@ -704,12 +689,6 @@
     <t>158,2757 mm</t>
   </si>
   <si>
-    <t>180,9555 mm</t>
-  </si>
-  <si>
-    <t>204,4237 mm</t>
-  </si>
-  <si>
     <t>45,4591 mm</t>
   </si>
   <si>
@@ -1109,18 +1088,6 @@
     <t>-179,7 deg</t>
   </si>
   <si>
-    <t>188,5597 mm</t>
-  </si>
-  <si>
-    <t>208,5115 mm</t>
-  </si>
-  <si>
-    <t>179,5409 mm</t>
-  </si>
-  <si>
-    <t>200,0604 mm</t>
-  </si>
-  <si>
     <t>180,5703 mm</t>
   </si>
   <si>
@@ -1149,6 +1116,66 @@
   </si>
   <si>
     <t>91,875 mm</t>
+  </si>
+  <si>
+    <t>181,2172 mm</t>
+  </si>
+  <si>
+    <t>204,25 mm</t>
+  </si>
+  <si>
+    <t>45,7009 mm</t>
+  </si>
+  <si>
+    <t>46,5009 mm</t>
+  </si>
+  <si>
+    <t>184,7838 mm</t>
+  </si>
+  <si>
+    <t>205,5171 mm</t>
+  </si>
+  <si>
+    <t>Ball 9</t>
+  </si>
+  <si>
+    <t>Ball 8</t>
+  </si>
+  <si>
+    <t>Ball 4</t>
+  </si>
+  <si>
+    <t>Ball w</t>
+  </si>
+  <si>
+    <t>171,8906 mm</t>
+  </si>
+  <si>
+    <t>195,9607 mm</t>
+  </si>
+  <si>
+    <t>19,6236 mm</t>
+  </si>
+  <si>
+    <t>24,7691 mm</t>
+  </si>
+  <si>
+    <t>41,3 deg</t>
+  </si>
+  <si>
+    <t>178,2415 mm</t>
+  </si>
+  <si>
+    <t>199,0955 mm</t>
+  </si>
+  <si>
+    <t>21,4358 mm</t>
+  </si>
+  <si>
+    <t>24,7411 mm</t>
+  </si>
+  <si>
+    <t>28 deg</t>
   </si>
 </sst>
 </file>
@@ -1502,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A186" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H189" sqref="H189:H196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1544,16 +1571,16 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="G2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="H2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
@@ -1582,16 +1609,16 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="G3" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="H3" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
@@ -1618,16 +1645,16 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="G4" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="H4" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -1651,16 +1678,16 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="G5" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="H5" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -1684,16 +1711,16 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="H6" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -1717,16 +1744,16 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="G7" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="H7" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -1741,16 +1768,16 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="G8" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" t="s">
+        <v>302</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="H8" t="s">
-        <v>309</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>318</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -1764,23 +1791,25 @@
       <c r="A9" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="G9" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H9" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1795,22 +1824,22 @@
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="G10" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="H10" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -1825,22 +1854,22 @@
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="G11" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="H11" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -1855,22 +1884,22 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="G12" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="H12" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="I12" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="M12" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1882,7 +1911,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1890,36 +1919,42 @@
         <v>141</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; A9 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; A9 &amp; """, Target = """ &amp; B9 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B10,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B11,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B12,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B13,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B14,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 1", PixelCenter = new PointF(111.78f, 166.22f), PixelSize = new SizeF(175.02f, 176.32f), Degrees = -179.50f },</v>
+        <v>new BallPosition { Name = "Ball 1", Target = "Ball 1", PixelCenter = new PointF(111.78f, 166.22f), PixelSize = new SizeF(175.02f, 176.32f), Degrees = -179.50f },</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="U16" s="2"/>
@@ -1929,28 +1964,28 @@
         <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M17" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; A16 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; A16 &amp; """, Target = """ &amp; B16 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 9a", PixelCenter = new PointF(326.64f, 247.57f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
+        <v>new BallPosition { Name = "Ball 9a", Target = "Ball 9", PixelCenter = new PointF(326.64f, 247.57f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1958,28 +1993,28 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G18" t="s">
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M18" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; D16 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; D16 &amp; """, Target = """ &amp; E16 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 9b", PixelCenter = new PointF(337.32f, 267.88f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
+        <v>new BallPosition { Name = "Ball 9b", Target = "Ball 9", PixelCenter = new PointF(337.32f, 267.88f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1987,28 +2022,28 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="M19" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; G16 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; G16 &amp; """, Target = """ &amp; H16 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(H17,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(H18,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 9c", PixelCenter = new PointF(340.62f, 297.17f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
+        <v>new BallPosition { Name = "Ball 9c", Target = "Ball 9", PixelCenter = new PointF(340.62f, 297.17f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2016,28 +2051,28 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="M20" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; A23 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; A23 &amp; """, Target = """ &amp; B23 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B24,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B25,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B26,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B27,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 8a", PixelCenter = new PointF(513.15f, 187.86f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
+        <v>new BallPosition { Name = "Ball 8a", Target = "Ball 8", PixelCenter = new PointF(513.15f, 187.86f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2045,61 +2080,65 @@
         <v>141</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D21" t="s">
         <v>141</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G21" t="s">
         <v>141</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="M21" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; D23 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; D23 &amp; """, Target = """ &amp; E23 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E24,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E25,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E26,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E27,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 8b", PixelCenter = new PointF(495.39f, 193.06f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
+        <v>new BallPosition { Name = "Ball 8b", Target = "Ball 8", PixelCenter = new PointF(495.39f, 193.06f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M22" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; A30 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; A30 &amp; """, Target = """ &amp; B30 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B31,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B32,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B33,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B34,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B35,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 4a", PixelCenter = new PointF(675.32f, 122.76f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = -179.70f },</v>
+        <v>new BallPosition { Name = "Ball 4a", Target = "Ball 4", PixelCenter = new PointF(676.31f, 123.41f), PixelSize = new SizeF(172.73f, 175.75f), Degrees = -179.70f },</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="1" t="s">
+        <v>371</v>
+      </c>
       <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="1" t="s">
+        <v>371</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="M23" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; D30 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; D30 &amp; """, Target = """ &amp; E30 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E31,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E32,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E33,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E34,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E35,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball 4b", PixelCenter = new PointF(704.06f, 107.31f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = -179.70f },</v>
+        <v>new BallPosition { Name = "Ball 4b", Target = "Ball 4", PixelCenter = new PointF(689.79f, 118.62f), PixelSize = new SizeF(172.73f, 175.75f), Degrees = -179.70f },</v>
       </c>
       <c r="Q23" s="2"/>
     </row>
@@ -2108,7 +2147,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D24" t="s">
         <v>2</v>
@@ -2117,13 +2156,13 @@
         <v>175</v>
       </c>
       <c r="M24" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; A37 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; A37 &amp; """, Target = """ &amp; B37 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B38,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B39,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B40,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B41,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B42,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball wa", PixelCenter = new PointF(295.17f, 550.50f), PixelSize = new SizeF(177.64f, 177.64f), Degrees = 0.00f },</v>
+        <v>new BallPosition { Name = "Ball wa", Target = "Ball w", PixelCenter = new PointF(295.17f, 550.50f), PixelSize = new SizeF(177.64f, 177.64f), Degrees = 0.00f },</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -2131,23 +2170,23 @@
         <v>3</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="5" t="str">
-        <f>"new Ball { Name = """ &amp; D37 &amp; """, PixelCenter = new PointF(" &amp;
+        <f>"new BallPosition { Name = """ &amp; D37 &amp; """, Target = """ &amp; E37 &amp; """, PixelCenter = new PointF(" &amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E38,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E39,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), PixelSize = new SizeF(" &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E40,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E41,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E42,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new Ball { Name = "Ball wb", PixelCenter = new PointF(287.61f, 548.14f), PixelSize = new SizeF(177.64f, 177.64f), Degrees = 0.00f },</v>
+        <v>new BallPosition { Name = "Ball wb", Target = "Ball w", PixelCenter = new PointF(287.61f, 548.14f), PixelSize = new SizeF(177.64f, 177.64f), Degrees = 0.00f },</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -2155,13 +2194,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26"/>
@@ -2171,13 +2210,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27"/>
@@ -2187,13 +2226,13 @@
         <v>141</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D28" t="s">
         <v>141</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="I28" s="4"/>
       <c r="L28" s="2"/>
@@ -2205,14 +2244,18 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B30" s="5"/>
+        <v>351</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="C30" s="5"/>
       <c r="D30" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="E30" s="5"/>
+        <v>352</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="L30" s="2"/>
@@ -2223,13 +2266,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>226</v>
+        <v>364</v>
       </c>
       <c r="D31" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31"/>
@@ -2239,13 +2282,13 @@
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>227</v>
+        <v>365</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32"/>
@@ -2255,13 +2298,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33"/>
@@ -2271,13 +2314,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>229</v>
+        <v>367</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>229</v>
+        <v>367</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34"/>
@@ -2287,13 +2330,13 @@
         <v>141</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="D35" t="s">
         <v>141</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="I35" s="4"/>
       <c r="L35" s="2"/>
@@ -2301,27 +2344,31 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="B37" s="5"/>
+        <v>357</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>373</v>
+      </c>
       <c r="C37" s="5"/>
       <c r="D37" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="E37" s="5"/>
+        <v>358</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="D38" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2329,13 +2376,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2371,13 +2418,13 @@
         <v>141</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="D42" t="s">
         <v>141</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="F42" s="4"/>
       <c r="J42" s="4"/>
@@ -4727,7 +4774,7 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B144" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
@@ -4744,7 +4791,7 @@
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
       <c r="F144" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="G144" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
@@ -4769,13 +4816,13 @@
         <v>10</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F145" t="s">
         <v>10</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="K145" s="2"/>
       <c r="M145"/>
@@ -4785,13 +4832,13 @@
         <v>11</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="F146" t="s">
         <v>11</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="K146" s="2"/>
       <c r="M146"/>
@@ -4801,13 +4848,13 @@
         <v>4</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="F147" t="s">
         <v>4</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="K147" s="2"/>
       <c r="M147"/>
@@ -4817,13 +4864,13 @@
         <v>5</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F148" t="s">
         <v>5</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="K148" s="2"/>
       <c r="M148"/>
@@ -4833,7 +4880,7 @@
         <v>14</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C149">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B149,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4846,7 +4893,7 @@
         <v>14</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H149">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G149,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4863,7 +4910,7 @@
         <v>15</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C150">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B150,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4876,7 +4923,7 @@
         <v>15</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="H150">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G150,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4893,7 +4940,7 @@
         <v>16</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C151">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B151,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4906,7 +4953,7 @@
         <v>16</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H151">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G151,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4983,7 +5030,7 @@
         <v>19</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C154">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B154,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4996,7 +5043,7 @@
         <v>19</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="H154">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G154,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5013,7 +5060,7 @@
         <v>20</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C155">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B155,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5026,7 +5073,7 @@
         <v>20</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H155">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G155,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5043,7 +5090,7 @@
         <v>21</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C156">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B156,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5056,7 +5103,7 @@
         <v>21</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="H156">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G156,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5117,7 +5164,7 @@
         <v>10</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C162">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B162,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5130,7 +5177,7 @@
         <v>10</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="H162">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G162,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5158,7 +5205,7 @@
         <v>11</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C163">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B163,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5171,7 +5218,7 @@
         <v>11</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="H163">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G163,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5196,10 +5243,10 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C164">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B164,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5209,10 +5256,10 @@
         <v>6</v>
       </c>
       <c r="F164" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H164">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G164,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5222,7 +5269,7 @@
         <v>6</v>
       </c>
       <c r="K164" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L164" s="3" t="s">
         <v>150</v>
@@ -5237,10 +5284,10 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C165">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B165,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5250,10 +5297,10 @@
         <v>6</v>
       </c>
       <c r="F165" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="H165">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G165,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5263,7 +5310,7 @@
         <v>6</v>
       </c>
       <c r="K165" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="L165" s="3" t="s">
         <v>151</v>
@@ -5278,10 +5325,10 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5291,10 +5338,10 @@
         <v>6</v>
       </c>
       <c r="F166" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5304,10 +5351,10 @@
         <v>6</v>
       </c>
       <c r="K166" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="L166" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="M166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5319,10 +5366,10 @@
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5332,10 +5379,10 @@
         <v>6</v>
       </c>
       <c r="F167" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="H167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5345,10 +5392,10 @@
         <v>6</v>
       </c>
       <c r="K167" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="L167" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="M167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5363,7 +5410,7 @@
         <v>141</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C168">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B168,".",",")," deg",""))</f>
@@ -5438,7 +5485,7 @@
         <v>10</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C171">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B171,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5451,7 +5498,7 @@
         <v>10</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H171">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G171,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5479,7 +5526,7 @@
         <v>11</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C172">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B172,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5492,7 +5539,7 @@
         <v>11</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H172">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G172,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5517,10 +5564,10 @@
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C173">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B173,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5530,10 +5577,10 @@
         <v>6</v>
       </c>
       <c r="F173" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H173">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G173,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5543,7 +5590,7 @@
         <v>6</v>
       </c>
       <c r="K173" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L173" s="3" t="s">
         <v>144</v>
@@ -5558,10 +5605,10 @@
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C174">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B174,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5571,10 +5618,10 @@
         <v>6</v>
       </c>
       <c r="F174" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H174">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G174,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5584,7 +5631,7 @@
         <v>6</v>
       </c>
       <c r="K174" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="L174" s="3" t="s">
         <v>155</v>
@@ -5599,10 +5646,10 @@
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5612,10 +5659,10 @@
         <v>6</v>
       </c>
       <c r="F175" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="H175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5625,10 +5672,10 @@
         <v>6</v>
       </c>
       <c r="K175" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="L175" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="M175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5640,10 +5687,10 @@
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5653,10 +5700,10 @@
         <v>6</v>
       </c>
       <c r="F176" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5666,10 +5713,10 @@
         <v>6</v>
       </c>
       <c r="K176" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="L176" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="M176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5684,7 +5731,7 @@
         <v>141</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C177">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B177,".",",")," deg",""))</f>
@@ -5759,7 +5806,7 @@
         <v>10</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C180">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B180,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5772,7 +5819,7 @@
         <v>10</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H180">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G180,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5800,7 +5847,7 @@
         <v>11</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C181">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B181,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5813,7 +5860,7 @@
         <v>11</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H181">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G181,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5838,10 +5885,10 @@
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C182">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B182,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5851,10 +5898,10 @@
         <v>6</v>
       </c>
       <c r="F182" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H182">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G182,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5864,7 +5911,7 @@
         <v>6</v>
       </c>
       <c r="K182" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L182" s="3" t="s">
         <v>159</v>
@@ -5879,10 +5926,10 @@
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C183">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B183,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5892,10 +5939,10 @@
         <v>6</v>
       </c>
       <c r="F183" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H183">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G183,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5920,10 +5967,10 @@
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5933,10 +5980,10 @@
         <v>6</v>
       </c>
       <c r="F184" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5946,10 +5993,10 @@
         <v>6</v>
       </c>
       <c r="K184" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="L184" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="M184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5961,10 +6008,10 @@
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5974,10 +6021,10 @@
         <v>6</v>
       </c>
       <c r="F185" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5987,10 +6034,10 @@
         <v>6</v>
       </c>
       <c r="K185" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="L185" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="M185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -6112,7 +6159,7 @@
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E208,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E205,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E206,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
-        <v>new Number { Target = "Ball 4b", PixelCenter = new PointF(669.97f, 139.25f), PixelSize = new SizeF(74.17f, 93.62f), Degrees = 41.30f, OrientStart = new PointF(653.94f, 144.58f), OrientEnd = new PointF(644.95f, 184.83f) },</v>
+        <v>new Number { Target = "Ball 4b", PixelCenter = new PointF(665.06f, 142.90f), PixelSize = new SizeF(81.02f, 93.51f), Degrees = 28.00f, OrientStart = new PointF(653.94f, 144.58f), OrientEnd = new PointF(644.95f, 184.83f) },</v>
       </c>
       <c r="K191" s="2"/>
       <c r="M191"/>
@@ -6165,10 +6212,10 @@
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H194" s="7" t="str">
         <f>"new Number { Target = """ &amp; A221 &amp; """, PixelCenter = new PointF("&amp;
@@ -6188,10 +6235,10 @@
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H195" s="7" t="str">
         <f>"new Number { Target = """ &amp; D221 &amp; """, PixelCenter = new PointF("&amp;
@@ -6211,10 +6258,10 @@
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H196" s="7" t="str">
         <f>"new Number { Target = """ &amp; G221 &amp; """, PixelCenter = new PointF("&amp;
@@ -6234,10 +6281,10 @@
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="K197" s="2"/>
       <c r="M197"/>
@@ -6248,11 +6295,11 @@
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B199"/>
       <c r="D199" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="I199" s="2"/>
       <c r="M199"/>
@@ -6262,13 +6309,13 @@
         <v>10</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>183</v>
+        <v>374</v>
       </c>
       <c r="D200" t="s">
         <v>10</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>363</v>
+        <v>379</v>
       </c>
       <c r="I200" s="2"/>
       <c r="M200"/>
@@ -6278,13 +6325,13 @@
         <v>11</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>184</v>
+        <v>375</v>
       </c>
       <c r="D201" t="s">
         <v>11</v>
       </c>
       <c r="E201" s="3" t="s">
-        <v>364</v>
+        <v>380</v>
       </c>
       <c r="I201" s="2"/>
       <c r="M201"/>
@@ -6294,13 +6341,13 @@
         <v>4</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>181</v>
+        <v>376</v>
       </c>
       <c r="D202" t="s">
         <v>4</v>
       </c>
       <c r="E202" s="3" t="s">
-        <v>181</v>
+        <v>381</v>
       </c>
       <c r="I202" s="2"/>
       <c r="M202"/>
@@ -6310,13 +6357,13 @@
         <v>5</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>185</v>
+        <v>377</v>
       </c>
       <c r="D203" t="s">
         <v>5</v>
       </c>
       <c r="E203" s="3" t="s">
-        <v>185</v>
+        <v>382</v>
       </c>
       <c r="F203" s="5"/>
       <c r="I203" s="2"/>
@@ -6327,77 +6374,77 @@
         <v>141</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>182</v>
+        <v>378</v>
       </c>
       <c r="D204" t="s">
         <v>141</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>182</v>
+        <v>383</v>
       </c>
       <c r="I204" s="2"/>
       <c r="M204"/>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D205" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I205" s="2"/>
       <c r="M205"/>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D206" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E206" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I206" s="2"/>
       <c r="M206"/>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D207" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I207" s="2"/>
       <c r="M207"/>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D208" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I208" s="2"/>
       <c r="M208"/>
@@ -6422,13 +6469,13 @@
         <v>10</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D211" t="s">
         <v>10</v>
       </c>
       <c r="E211" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H211" s="5"/>
       <c r="I211" s="2"/>
@@ -6439,13 +6486,13 @@
         <v>11</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D212" t="s">
         <v>11</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H212" s="5"/>
       <c r="I212" s="2"/>
@@ -6456,13 +6503,13 @@
         <v>4</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D213" t="s">
         <v>4</v>
       </c>
       <c r="E213" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H213" s="5"/>
       <c r="I213" s="2"/>
@@ -6473,13 +6520,13 @@
         <v>5</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D214" t="s">
         <v>5</v>
       </c>
       <c r="E214" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H214" s="5"/>
       <c r="I214" s="2"/>
@@ -6490,13 +6537,13 @@
         <v>141</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D215" t="s">
         <v>141</v>
       </c>
       <c r="E215" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H215" s="5"/>
       <c r="I215" s="2"/>
@@ -6504,16 +6551,16 @@
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D216" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="F216" s="5"/>
       <c r="H216" s="5"/>
@@ -6522,16 +6569,16 @@
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D217" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E217" s="3" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="H217" s="5"/>
       <c r="I217" s="2"/>
@@ -6539,16 +6586,16 @@
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D218" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E218" s="3" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="H218" s="5"/>
       <c r="I218" s="2"/>
@@ -6556,16 +6603,16 @@
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D219" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H219" s="5"/>
       <c r="I219" s="2"/>
@@ -6596,19 +6643,19 @@
         <v>10</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D222" t="s">
         <v>10</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="G222" t="s">
         <v>10</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="I222" s="2"/>
       <c r="M222"/>
@@ -6618,19 +6665,19 @@
         <v>11</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D223" t="s">
         <v>11</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="G223" t="s">
         <v>11</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="I223" s="2"/>
       <c r="M223"/>
@@ -6640,19 +6687,19 @@
         <v>4</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D224" t="s">
         <v>4</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="G224" t="s">
         <v>4</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="I224" s="2"/>
       <c r="M224"/>
@@ -6662,19 +6709,19 @@
         <v>5</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D225" t="s">
         <v>5</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="G225" t="s">
         <v>5</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="I225" s="2"/>
       <c r="M225"/>
@@ -6684,84 +6731,84 @@
         <v>141</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D226" t="s">
         <v>141</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="G226" t="s">
         <v>141</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="I226" s="2"/>
       <c r="M226"/>
     </row>
     <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B227" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D227" t="s">
+        <v>185</v>
+      </c>
+      <c r="E227" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="D227" t="s">
-        <v>190</v>
-      </c>
-      <c r="E227" s="3" t="s">
-        <v>348</v>
-      </c>
       <c r="G227" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H227" s="3" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="M227"/>
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B228" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D228" t="s">
+        <v>186</v>
+      </c>
+      <c r="E228" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D228" t="s">
-        <v>191</v>
-      </c>
-      <c r="E228" s="3" t="s">
-        <v>349</v>
-      </c>
       <c r="G228" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="M228"/>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B229" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D229" t="s">
+        <v>187</v>
+      </c>
+      <c r="E229" s="3" t="s">
         <v>343</v>
-      </c>
-      <c r="D229" t="s">
-        <v>192</v>
-      </c>
-      <c r="E229" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="F229" s="5"/>
       <c r="G229" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H229" s="3" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="I229" s="5"/>
       <c r="J229" s="5"/>
@@ -6769,22 +6816,22 @@
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B230" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D230" t="s">
+        <v>188</v>
+      </c>
+      <c r="E230" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="D230" t="s">
-        <v>193</v>
-      </c>
-      <c r="E230" s="3" t="s">
-        <v>351</v>
-      </c>
       <c r="G230" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H230" s="3" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="M230"/>
     </row>
@@ -6814,20 +6861,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B144:D144"/>
-    <mergeCell ref="G144:I144"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="G130:I130"/>
-    <mergeCell ref="L161:N161"/>
-    <mergeCell ref="L170:N170"/>
-    <mergeCell ref="L179:N179"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="G88:I88"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="G116:I116"/>
-    <mergeCell ref="G102:I102"/>
-    <mergeCell ref="B74:D74"/>
     <mergeCell ref="G60:I60"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="G46:I46"/>
@@ -6841,6 +6874,15 @@
     <mergeCell ref="I8:L8"/>
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
+    <mergeCell ref="L170:N170"/>
+    <mergeCell ref="L179:N179"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="G88:I88"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="G116:I116"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="B74:D74"/>
     <mergeCell ref="B88:D88"/>
     <mergeCell ref="B161:D161"/>
     <mergeCell ref="B170:D170"/>
@@ -6848,6 +6890,11 @@
     <mergeCell ref="G161:I161"/>
     <mergeCell ref="G170:I170"/>
     <mergeCell ref="G179:I179"/>
+    <mergeCell ref="B144:D144"/>
+    <mergeCell ref="G144:I144"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="G130:I130"/>
+    <mergeCell ref="L161:N161"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Refined positions and animations
</commit_message>
<xml_diff>
--- a/Documentation/Original.xlsx
+++ b/Documentation/Original.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="387">
   <si>
     <t>Pixelwidth</t>
   </si>
@@ -665,48 +665,6 @@
     <t>-179,5 deg</t>
   </si>
   <si>
-    <t>88,6996 mm</t>
-  </si>
-  <si>
-    <t>171,4001 mm</t>
-  </si>
-  <si>
-    <t>45,8009 mm</t>
-  </si>
-  <si>
-    <t>46,8016 mm</t>
-  </si>
-  <si>
-    <t>91,5255 mm</t>
-  </si>
-  <si>
-    <t>166,0257 mm</t>
-  </si>
-  <si>
-    <t>92,4005 mm</t>
-  </si>
-  <si>
-    <t>158,2757 mm</t>
-  </si>
-  <si>
-    <t>45,4591 mm</t>
-  </si>
-  <si>
-    <t>46,7445 mm</t>
-  </si>
-  <si>
-    <t>167 deg</t>
-  </si>
-  <si>
-    <t>138,0482 mm</t>
-  </si>
-  <si>
-    <t>187,1973 mm</t>
-  </si>
-  <si>
-    <t>185,8214 mm</t>
-  </si>
-  <si>
     <t>23,1177 mm</t>
   </si>
   <si>
@@ -926,12 +884,6 @@
     <t>8,2 mm</t>
   </si>
   <si>
-    <t>24,3 mm</t>
-  </si>
-  <si>
-    <t>201,2 mm</t>
-  </si>
-  <si>
     <t>5,4 mm</t>
   </si>
   <si>
@@ -962,12 +914,6 @@
     <t>Lightest part of Ball 4</t>
   </si>
   <si>
-    <t>155,0143 mm</t>
-  </si>
-  <si>
-    <t>176,8714 mm</t>
-  </si>
-  <si>
     <t>82,8429 mm</t>
   </si>
   <si>
@@ -1013,72 +959,9 @@
     <t>194,8 mm</t>
   </si>
   <si>
-    <t>78,7338 mm</t>
-  </si>
-  <si>
-    <t>181,5186 mm</t>
-  </si>
-  <si>
-    <t>24 mm</t>
-  </si>
-  <si>
-    <t>15,2398 mm</t>
-  </si>
-  <si>
-    <t>41 deg</t>
-  </si>
-  <si>
-    <t>82,25 mm</t>
-  </si>
-  <si>
-    <t>178,5 mm</t>
-  </si>
-  <si>
-    <t>77,05 mm</t>
-  </si>
-  <si>
-    <t>186,8 mm</t>
-  </si>
-  <si>
-    <t>88,1052 mm</t>
-  </si>
-  <si>
-    <t>167,0008 mm</t>
-  </si>
-  <si>
-    <t>30 deg</t>
-  </si>
-  <si>
-    <t>92,375 mm</t>
-  </si>
-  <si>
-    <t>168,125 mm</t>
-  </si>
-  <si>
     <t>87 mm</t>
   </si>
   <si>
-    <t>177,5 mm</t>
-  </si>
-  <si>
-    <t>90,1225 mm</t>
-  </si>
-  <si>
-    <t>162,9565 mm</t>
-  </si>
-  <si>
-    <t>88,25 mm</t>
-  </si>
-  <si>
-    <t>157 mm</t>
-  </si>
-  <si>
-    <t>90,725 mm</t>
-  </si>
-  <si>
-    <t>167,375 mm</t>
-  </si>
-  <si>
     <t>Ball 4a</t>
   </si>
   <si>
@@ -1088,15 +971,6 @@
     <t>-179,7 deg</t>
   </si>
   <si>
-    <t>180,5703 mm</t>
-  </si>
-  <si>
-    <t>192,0997 mm</t>
-  </si>
-  <si>
-    <t>182,9503 mm</t>
-  </si>
-  <si>
     <t>Ball wa</t>
   </si>
   <si>
@@ -1176,6 +1050,141 @@
   </si>
   <si>
     <t>28 deg</t>
+  </si>
+  <si>
+    <t>91,9 mm</t>
+  </si>
+  <si>
+    <t>158,575 mm</t>
+  </si>
+  <si>
+    <t>44,8 mm</t>
+  </si>
+  <si>
+    <t>46,4 mm</t>
+  </si>
+  <si>
+    <t>92,8533 mm</t>
+  </si>
+  <si>
+    <t>163,2667 mm</t>
+  </si>
+  <si>
+    <t>88,28 mm</t>
+  </si>
+  <si>
+    <t>171,56 mm</t>
+  </si>
+  <si>
+    <t>88,4426 mm</t>
+  </si>
+  <si>
+    <t>156,9016 mm</t>
+  </si>
+  <si>
+    <t>23,9927 mm</t>
+  </si>
+  <si>
+    <t>22,3008 mm</t>
+  </si>
+  <si>
+    <t>-12 deg</t>
+  </si>
+  <si>
+    <t>85,8667 mm</t>
+  </si>
+  <si>
+    <t>155,2 mm</t>
+  </si>
+  <si>
+    <t>92,2 mm</t>
+  </si>
+  <si>
+    <t>159,6 mm</t>
+  </si>
+  <si>
+    <t>89,6361 mm</t>
+  </si>
+  <si>
+    <t>163,0572 mm</t>
+  </si>
+  <si>
+    <t>25,2516 mm</t>
+  </si>
+  <si>
+    <t>-24 deg</t>
+  </si>
+  <si>
+    <t>165,6667 mm</t>
+  </si>
+  <si>
+    <t>93 mm</t>
+  </si>
+  <si>
+    <t>171,6 mm</t>
+  </si>
+  <si>
+    <t>79,3917 mm</t>
+  </si>
+  <si>
+    <t>180,1437 mm</t>
+  </si>
+  <si>
+    <t>18,64 mm</t>
+  </si>
+  <si>
+    <t>24,28 mm</t>
+  </si>
+  <si>
+    <t>-53 deg</t>
+  </si>
+  <si>
+    <t>77,0667 mm</t>
+  </si>
+  <si>
+    <t>178,1333 mm</t>
+  </si>
+  <si>
+    <t>81 mm</t>
+  </si>
+  <si>
+    <t>184,4 mm</t>
+  </si>
+  <si>
+    <t>127,5 mm</t>
+  </si>
+  <si>
+    <t>177,3 mm</t>
+  </si>
+  <si>
+    <t>134,1 mm</t>
+  </si>
+  <si>
+    <t>186,25 mm</t>
+  </si>
+  <si>
+    <t>44,95 mm</t>
+  </si>
+  <si>
+    <t>45,75 mm</t>
+  </si>
+  <si>
+    <t>138,075 mm</t>
+  </si>
+  <si>
+    <t>189,6083 mm</t>
+  </si>
+  <si>
+    <t>163,4429 mm</t>
+  </si>
+  <si>
+    <t>180,1571 mm</t>
+  </si>
+  <si>
+    <t>30,2333 mm</t>
+  </si>
+  <si>
+    <t>205,2333 mm</t>
   </si>
 </sst>
 </file>
@@ -1529,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H189" sqref="H189:H196"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1571,16 +1580,16 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="G2" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="H2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>289</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>305</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
@@ -1609,16 +1618,16 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>312</v>
+        <v>383</v>
       </c>
       <c r="G3" t="s">
-        <v>313</v>
+        <v>384</v>
       </c>
       <c r="H3" t="s">
+        <v>276</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>290</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>306</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
@@ -1628,7 +1637,7 @@
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(F3,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G3,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".") &amp; "f), Radius = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H3,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f }, // " &amp; I3</f>
-        <v>new ColorRef { PixelCenter = new PointF(577.27f, 226.89f), Radius = 24.94f }, // Darkest part of the cloth (ambient color)</v>
+        <v>new ColorRef { PixelCenter = new PointF(609.13f, 214.47f), Radius = 24.94f }, // Darkest part of the cloth (ambient color)</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -1645,16 +1654,16 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="G4" t="s">
+        <v>278</v>
+      </c>
+      <c r="H4" t="s">
+        <v>279</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>292</v>
-      </c>
-      <c r="H4" t="s">
-        <v>293</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>308</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -1678,16 +1687,16 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="G5" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="H5" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -1711,16 +1720,16 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="G6" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="H6" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -1744,23 +1753,23 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>300</v>
+        <v>385</v>
       </c>
       <c r="G7" t="s">
-        <v>301</v>
+        <v>386</v>
       </c>
       <c r="H7" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>new ColorRef { PixelCenter = new PointF(83.24f, 134.94f), Radius = 20.41f }, // Lightest part of Ball 1</v>
+        <v>new ColorRef { PixelCenter = new PointF(105.66f, 119.70f), Radius = 20.41f }, // Lightest part of Ball 1</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1768,16 +1777,16 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="G8" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="H8" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -1800,16 +1809,16 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="G9" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="H9" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1830,16 +1839,16 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="G10" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="H10" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -1860,16 +1869,16 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="G11" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="H11" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -1890,16 +1899,16 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="G12" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="H12" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="I12" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="M12" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1927,21 +1936,21 @@
         <v>165</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
         <v>166</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="1" t="s">
         <v>167</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1964,19 +1973,19 @@
         <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>213</v>
+        <v>342</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>217</v>
+        <v>346</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>219</v>
+        <v>348</v>
       </c>
       <c r="M17" s="5" t="str">
         <f>"new BallPosition { Name = """ &amp; A16 &amp; """, Target = """ &amp; B16 &amp; """, PixelCenter = new PointF(" &amp;
@@ -1985,7 +1994,7 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new BallPosition { Name = "Ball 9a", Target = "Ball 9", PixelCenter = new PointF(326.64f, 247.57f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
+        <v>new BallPosition { Name = "Ball 9a", Target = "Ball 9", PixelCenter = new PointF(338.73f, 296.04f), PixelSize = new SizeF(169.32f, 175.37f), Degrees = 0.00f },</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1993,19 +2002,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>214</v>
+        <v>343</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>218</v>
+        <v>347</v>
       </c>
       <c r="G18" t="s">
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>220</v>
+        <v>349</v>
       </c>
       <c r="M18" s="5" t="str">
         <f>"new BallPosition { Name = """ &amp; D16 &amp; """, Target = """ &amp; E16 &amp; """, PixelCenter = new PointF(" &amp;
@@ -2014,7 +2023,7 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new BallPosition { Name = "Ball 9b", Target = "Ball 9", PixelCenter = new PointF(337.32f, 267.88f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
+        <v>new BallPosition { Name = "Ball 9b", Target = "Ball 9", PixelCenter = new PointF(342.34f, 278.31f), PixelSize = new SizeF(169.32f, 175.37f), Degrees = 0.00f },</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2022,19 +2031,19 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>215</v>
+        <v>344</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>215</v>
+        <v>344</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>215</v>
+        <v>344</v>
       </c>
       <c r="M19" s="5" t="str">
         <f>"new BallPosition { Name = """ &amp; G16 &amp; """, Target = """ &amp; H16 &amp; """, PixelCenter = new PointF(" &amp;
@@ -2043,7 +2052,7 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H19,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H20,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(H21,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new BallPosition { Name = "Ball 9c", Target = "Ball 9", PixelCenter = new PointF(340.62f, 297.17f), PixelSize = new SizeF(173.11f, 176.89f), Degrees = -179.50f },</v>
+        <v>new BallPosition { Name = "Ball 9c", Target = "Ball 9", PixelCenter = new PointF(325.05f, 246.97f), PixelSize = new SizeF(169.32f, 175.37f), Degrees = 0.00f },</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2051,19 +2060,19 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>216</v>
+        <v>345</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>216</v>
+        <v>345</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>216</v>
+        <v>345</v>
       </c>
       <c r="M20" s="5" t="str">
         <f>"new BallPosition { Name = """ &amp; A23 &amp; """, Target = """ &amp; B23 &amp; """, PixelCenter = new PointF(" &amp;
@@ -2072,7 +2081,7 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B26,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B27,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(B28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new BallPosition { Name = "Ball 8a", Target = "Ball 8", PixelCenter = new PointF(513.15f, 187.86f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
+        <v>new BallPosition { Name = "Ball 8a", Target = "Ball 8", PixelCenter = new PointF(495.39f, 191.44f), PixelSize = new SizeF(169.89f, 172.91f), Degrees = 0.00f },</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2080,19 +2089,19 @@
         <v>141</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>212</v>
+        <v>319</v>
       </c>
       <c r="D21" t="s">
         <v>141</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>212</v>
+        <v>319</v>
       </c>
       <c r="G21" t="s">
         <v>141</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>212</v>
+        <v>319</v>
       </c>
       <c r="M21" s="5" t="str">
         <f>"new BallPosition { Name = """ &amp; D23 &amp; """, Target = """ &amp; E23 &amp; """, PixelCenter = new PointF(" &amp;
@@ -2101,7 +2110,7 @@
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E26,".",",")," mm",""))*$B$2/$B$6, "0,00"),",",".") &amp; "f, " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E27,".",",")," mm",""))*$B$3/$B$7,"0,00"),",",".") &amp; "f), Degrees = " &amp;
 SUBSTITUTE(TEXT(VALUE(SUBSTITUTE(SUBSTITUTE(E28,".",",")," deg","")),"0,00"),",",".") &amp; "f },"</f>
-        <v>new BallPosition { Name = "Ball 8b", Target = "Ball 8", PixelCenter = new PointF(495.39f, 193.06f), PixelSize = new SizeF(171.81f, 176.67f), Degrees = 167.00f },</v>
+        <v>new BallPosition { Name = "Ball 8b", Target = "Ball 8", PixelCenter = new PointF(513.25f, 178.75f), PixelSize = new SizeF(169.89f, 172.91f), Degrees = 0.00f },</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2120,14 +2129,14 @@
         <v>168</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>371</v>
+        <v>329</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>371</v>
+        <v>329</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -2147,13 +2156,13 @@
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>224</v>
+        <v>175</v>
       </c>
       <c r="D24" t="s">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>175</v>
+        <v>381</v>
       </c>
       <c r="M24" s="5" t="str">
         <f>"new BallPosition { Name = """ &amp; A37 &amp; """, Target = """ &amp; B37 &amp; """, PixelCenter = new PointF(" &amp;
@@ -2170,13 +2179,13 @@
         <v>3</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>225</v>
+        <v>378</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>226</v>
+        <v>382</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="5" t="str">
@@ -2194,13 +2203,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>221</v>
+        <v>379</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>221</v>
+        <v>379</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26"/>
@@ -2210,13 +2219,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>222</v>
+        <v>380</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>222</v>
+        <v>380</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27"/>
@@ -2226,13 +2235,13 @@
         <v>141</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>223</v>
+        <v>319</v>
       </c>
       <c r="D28" t="s">
         <v>141</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>223</v>
+        <v>319</v>
       </c>
       <c r="I28" s="4"/>
       <c r="L28" s="2"/>
@@ -2244,17 +2253,17 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>351</v>
+        <v>312</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>372</v>
+        <v>330</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="1" t="s">
-        <v>352</v>
+        <v>313</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>372</v>
+        <v>330</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2266,13 +2275,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="D31" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>368</v>
+        <v>326</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31"/>
@@ -2282,13 +2291,13 @@
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>369</v>
+        <v>327</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32"/>
@@ -2298,13 +2307,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>366</v>
+        <v>324</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>366</v>
+        <v>324</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33"/>
@@ -2314,13 +2323,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>367</v>
+        <v>325</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>367</v>
+        <v>325</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34"/>
@@ -2330,13 +2339,13 @@
         <v>141</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>353</v>
+        <v>314</v>
       </c>
       <c r="D35" t="s">
         <v>141</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>353</v>
+        <v>314</v>
       </c>
       <c r="I35" s="4"/>
       <c r="L35" s="2"/>
@@ -2344,17 +2353,17 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>373</v>
+        <v>331</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="1" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>373</v>
+        <v>331</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -2362,13 +2371,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
       <c r="D38" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>362</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2376,13 +2385,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2418,13 +2427,13 @@
         <v>141</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>361</v>
+        <v>319</v>
       </c>
       <c r="D42" t="s">
         <v>141</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>361</v>
+        <v>319</v>
       </c>
       <c r="F42" s="4"/>
       <c r="J42" s="4"/>
@@ -4774,7 +4783,7 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="B144" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
@@ -4791,7 +4800,7 @@
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
       <c r="F144" s="1" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G144" s="8" t="str">
         <f>"new PointF[4] { new PointF (" &amp;
@@ -4816,13 +4825,13 @@
         <v>10</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="F145" t="s">
         <v>10</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="K145" s="2"/>
       <c r="M145"/>
@@ -4832,13 +4841,13 @@
         <v>11</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="F146" t="s">
         <v>11</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="K146" s="2"/>
       <c r="M146"/>
@@ -4848,13 +4857,13 @@
         <v>4</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="F147" t="s">
         <v>4</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="K147" s="2"/>
       <c r="M147"/>
@@ -4864,13 +4873,13 @@
         <v>5</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="F148" t="s">
         <v>5</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="K148" s="2"/>
       <c r="M148"/>
@@ -4880,7 +4889,7 @@
         <v>14</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="C149">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B149,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4893,7 +4902,7 @@
         <v>14</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="H149">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G149,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4910,7 +4919,7 @@
         <v>15</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="C150">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B150,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4923,7 +4932,7 @@
         <v>15</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="H150">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G150,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -4940,7 +4949,7 @@
         <v>16</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C151">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B151,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -4953,7 +4962,7 @@
         <v>16</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="H151">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G151,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5030,7 +5039,7 @@
         <v>19</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C154">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B154,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5043,7 +5052,7 @@
         <v>19</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="H154">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G154,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5060,7 +5069,7 @@
         <v>20</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C155">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B155,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5073,7 +5082,7 @@
         <v>20</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H155">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G145,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G147,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G155,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5090,7 +5099,7 @@
         <v>21</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C156">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(B148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(B156,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5103,7 +5112,7 @@
         <v>21</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="H156">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G146,".",",")," mm",""))-VALUE(SUBSTITUTE(SUBSTITUTE(G148,".",",")," mm",""))/2+VALUE(SUBSTITUTE(SUBSTITUTE(G156,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5164,7 +5173,7 @@
         <v>10</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C162">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B162,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5177,7 +5186,7 @@
         <v>10</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="H162">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G162,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5205,7 +5214,7 @@
         <v>11</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C163">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B163,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5218,7 +5227,7 @@
         <v>11</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="H163">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G163,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5243,10 +5252,10 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C164">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B164,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5256,10 +5265,10 @@
         <v>6</v>
       </c>
       <c r="F164" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="H164">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G164,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5269,7 +5278,7 @@
         <v>6</v>
       </c>
       <c r="K164" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="L164" s="3" t="s">
         <v>150</v>
@@ -5284,10 +5293,10 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C165">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B165,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5297,10 +5306,10 @@
         <v>6</v>
       </c>
       <c r="F165" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="H165">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G165,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5310,7 +5319,7 @@
         <v>6</v>
       </c>
       <c r="K165" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="L165" s="3" t="s">
         <v>151</v>
@@ -5325,10 +5334,10 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5338,10 +5347,10 @@
         <v>6</v>
       </c>
       <c r="F166" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="H166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5351,10 +5360,10 @@
         <v>6</v>
       </c>
       <c r="K166" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="L166" s="3" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="M166">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L166,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5366,10 +5375,10 @@
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5379,10 +5388,10 @@
         <v>6</v>
       </c>
       <c r="F167" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="H167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5392,10 +5401,10 @@
         <v>6</v>
       </c>
       <c r="K167" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="L167" s="3" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="M167">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L167,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5410,7 +5419,7 @@
         <v>141</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C168">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B168,".",",")," deg",""))</f>
@@ -5485,7 +5494,7 @@
         <v>10</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="C171">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B171,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5498,7 +5507,7 @@
         <v>10</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="H171">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G171,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5526,7 +5535,7 @@
         <v>11</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="C172">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B172,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5539,7 +5548,7 @@
         <v>11</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="H172">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G172,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5564,10 +5573,10 @@
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="C173">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B173,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5577,10 +5586,10 @@
         <v>6</v>
       </c>
       <c r="F173" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="H173">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G173,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5590,7 +5599,7 @@
         <v>6</v>
       </c>
       <c r="K173" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="L173" s="3" t="s">
         <v>144</v>
@@ -5605,10 +5614,10 @@
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C174">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B174,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5618,10 +5627,10 @@
         <v>6</v>
       </c>
       <c r="F174" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="H174">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G174,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5631,7 +5640,7 @@
         <v>6</v>
       </c>
       <c r="K174" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="L174" s="3" t="s">
         <v>155</v>
@@ -5646,10 +5655,10 @@
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="C175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5659,10 +5668,10 @@
         <v>6</v>
       </c>
       <c r="F175" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="H175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5672,10 +5681,10 @@
         <v>6</v>
       </c>
       <c r="K175" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="L175" s="3" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="M175">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L175,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5687,10 +5696,10 @@
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5700,10 +5709,10 @@
         <v>6</v>
       </c>
       <c r="F176" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="H176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5713,10 +5722,10 @@
         <v>6</v>
       </c>
       <c r="K176" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="L176" s="3" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="M176">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L176,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5731,7 +5740,7 @@
         <v>141</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C177">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B177,".",",")," deg",""))</f>
@@ -5806,7 +5815,7 @@
         <v>10</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="C180">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(B180,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5819,7 +5828,7 @@
         <v>10</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="H180">
         <f>(VALUE(SUBSTITUTE(SUBSTITUTE(G180,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6</f>
@@ -5847,7 +5856,7 @@
         <v>11</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C181">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B181,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5860,7 +5869,7 @@
         <v>11</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="H181">
         <f>$B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(G181,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7</f>
@@ -5885,10 +5894,10 @@
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C182">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B182,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5898,10 +5907,10 @@
         <v>6</v>
       </c>
       <c r="F182" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="H182">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G182,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5911,7 +5920,7 @@
         <v>6</v>
       </c>
       <c r="K182" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="L182" s="3" t="s">
         <v>159</v>
@@ -5926,10 +5935,10 @@
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C183">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B183,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5939,10 +5948,10 @@
         <v>6</v>
       </c>
       <c r="F183" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="H183">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G183,".",",")," mm",""))*$B$3/$B$7</f>
@@ -5967,10 +5976,10 @@
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5980,10 +5989,10 @@
         <v>6</v>
       </c>
       <c r="F184" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="H184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -5993,10 +6002,10 @@
         <v>6</v>
       </c>
       <c r="K184" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="L184" s="3" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="M184">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L184,".",",")," mm",""))*$B$2/$B$6</f>
@@ -6008,10 +6017,10 @@
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -6021,10 +6030,10 @@
         <v>6</v>
       </c>
       <c r="F185" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="H185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(G185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -6034,10 +6043,10 @@
         <v>6</v>
       </c>
       <c r="K185" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="L185" s="3" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="M185">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(L185,".",",")," mm",""))*$B$3/$B$7</f>
@@ -6205,7 +6214,7 @@
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E219,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E216,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E217,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
-        <v>new Number { Target = "Ball 8b", PixelCenter = new PointF(486.89f, 205.26f), PixelSize = new SizeF(92.53f, 94.44f), Degrees = -4.80f, OrientStart = new PointF(682.86f, 189.74f), OrientEnd = new PointF(673.86f, 169.34f) },</v>
+        <v>new Number { Target = "Ball 8b", PixelCenter = new PointF(486.89f, 205.26f), PixelSize = new SizeF(92.53f, 94.44f), Degrees = -4.80f, OrientStart = new PointF(498.23f, 189.74f), OrientEnd = new PointF(473.28f, 225.27f) },</v>
       </c>
       <c r="K193" s="2"/>
       <c r="M193"/>
@@ -6228,7 +6237,7 @@
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B230,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(B227,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(B228,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
-        <v>new Number { Target = "Ball 9a", PixelCenter = new PointF(288.97f, 209.33f), PixelSize = new SizeF(90.71f, 57.60f), Degrees = 41.00f, OrientStart = new PointF(282.61f, 189.37f), OrientEnd = new PointF(302.26f, 220.74f) },</v>
+        <v>new Number { Target = "Ball 9a", PixelCenter = new PointF(325.66f, 302.37f), PixelSize = new SizeF(90.68f, 84.29f), Degrees = -12.00f, OrientStart = new PointF(339.87f, 292.17f), OrientEnd = new PointF(315.93f, 308.80f) },</v>
       </c>
       <c r="K194" s="2"/>
       <c r="M194"/>
@@ -6251,7 +6260,7 @@
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E230,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(E227,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(E228,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
-        <v>new Number { Target = "Ball 9b", PixelCenter = new PointF(324.39f, 264.20f), PixelSize = new SizeF(90.71f, 90.71f), Degrees = 30.00f, OrientStart = new PointF(320.21f, 224.52f), OrientEnd = new PointF(340.53f, 259.95f) },</v>
+        <v>new Number { Target = "Ball 9b", PixelCenter = new PointF(330.18f, 279.10f), PixelSize = new SizeF(90.68f, 95.44f), Degrees = -24.00f, OrientStart = new PointF(342.89f, 246.81f), OrientEnd = new PointF(320.21f, 269.24f) },</v>
       </c>
       <c r="K195" s="2"/>
       <c r="M195"/>
@@ -6274,7 +6283,7 @@
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(H230,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f), OrientEnd = new PointF("&amp;
 SUBSTITUTE(TEXT((VALUE(SUBSTITUTE(SUBSTITUTE(H227,".",",")," mm",""))-($B$4-$B$6/2))*$B$2/$B$6, "0,00"),",",".")&amp;"f, "&amp;
 SUBSTITUTE(TEXT($B$3-(VALUE(SUBSTITUTE(SUBSTITUTE(H228,".",",")," mm",""))-($B$5-$B$7/2))*$B$3/$B$7, "0,00"),",",".")&amp;"f) },"</f>
-        <v>new Number { Target = "Ball 9c", PixelCenter = new PointF(332.01f, 279.48f), PixelSize = new SizeF(90.71f, 90.71f), Degrees = 41.00f, OrientStart = new PointF(334.29f, 262.78f), OrientEnd = new PointF(324.94f, 302.00f) },</v>
+        <v>new Number { Target = "Ball 9c", PixelCenter = new PointF(291.46f, 214.52f), PixelSize = new SizeF(70.45f, 91.77f), Degrees = -53.00f, OrientStart = new PointF(297.54f, 198.44f), OrientEnd = new PointF(282.67f, 222.12f) },</v>
       </c>
       <c r="K196" s="2"/>
       <c r="M196"/>
@@ -6295,11 +6304,11 @@
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>351</v>
+        <v>312</v>
       </c>
       <c r="B199"/>
       <c r="D199" s="1" t="s">
-        <v>352</v>
+        <v>313</v>
       </c>
       <c r="I199" s="2"/>
       <c r="M199"/>
@@ -6309,13 +6318,13 @@
         <v>10</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>374</v>
+        <v>332</v>
       </c>
       <c r="D200" t="s">
         <v>10</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>379</v>
+        <v>337</v>
       </c>
       <c r="I200" s="2"/>
       <c r="M200"/>
@@ -6325,13 +6334,13 @@
         <v>11</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>375</v>
+        <v>333</v>
       </c>
       <c r="D201" t="s">
         <v>11</v>
       </c>
       <c r="E201" s="3" t="s">
-        <v>380</v>
+        <v>338</v>
       </c>
       <c r="I201" s="2"/>
       <c r="M201"/>
@@ -6341,13 +6350,13 @@
         <v>4</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>376</v>
+        <v>334</v>
       </c>
       <c r="D202" t="s">
         <v>4</v>
       </c>
       <c r="E202" s="3" t="s">
-        <v>381</v>
+        <v>339</v>
       </c>
       <c r="I202" s="2"/>
       <c r="M202"/>
@@ -6357,13 +6366,13 @@
         <v>5</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>377</v>
+        <v>335</v>
       </c>
       <c r="D203" t="s">
         <v>5</v>
       </c>
       <c r="E203" s="3" t="s">
-        <v>382</v>
+        <v>340</v>
       </c>
       <c r="F203" s="5"/>
       <c r="I203" s="2"/>
@@ -6374,13 +6383,13 @@
         <v>141</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>378</v>
+        <v>336</v>
       </c>
       <c r="D204" t="s">
         <v>141</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>383</v>
+        <v>341</v>
       </c>
       <c r="I204" s="2"/>
       <c r="M204"/>
@@ -6560,7 +6569,7 @@
         <v>185</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>354</v>
+        <v>375</v>
       </c>
       <c r="F216" s="5"/>
       <c r="H216" s="5"/>
@@ -6578,7 +6587,7 @@
         <v>186</v>
       </c>
       <c r="E217" s="3" t="s">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="H217" s="5"/>
       <c r="I217" s="2"/>
@@ -6595,7 +6604,7 @@
         <v>187</v>
       </c>
       <c r="E218" s="3" t="s">
-        <v>356</v>
+        <v>377</v>
       </c>
       <c r="H218" s="5"/>
       <c r="I218" s="2"/>
@@ -6643,19 +6652,19 @@
         <v>10</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>329</v>
+        <v>350</v>
       </c>
       <c r="D222" t="s">
         <v>10</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>338</v>
+        <v>359</v>
       </c>
       <c r="G222" t="s">
         <v>10</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="I222" s="2"/>
       <c r="M222"/>
@@ -6665,19 +6674,19 @@
         <v>11</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="D223" t="s">
         <v>11</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>339</v>
+        <v>360</v>
       </c>
       <c r="G223" t="s">
         <v>11</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="I223" s="2"/>
       <c r="M223"/>
@@ -6687,19 +6696,19 @@
         <v>4</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>331</v>
+        <v>352</v>
       </c>
       <c r="D224" t="s">
         <v>4</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>331</v>
+        <v>352</v>
       </c>
       <c r="G224" t="s">
         <v>4</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>331</v>
+        <v>368</v>
       </c>
       <c r="I224" s="2"/>
       <c r="M224"/>
@@ -6709,19 +6718,19 @@
         <v>5</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>332</v>
+        <v>353</v>
       </c>
       <c r="D225" t="s">
         <v>5</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>331</v>
+        <v>361</v>
       </c>
       <c r="G225" t="s">
         <v>5</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>331</v>
+        <v>369</v>
       </c>
       <c r="I225" s="2"/>
       <c r="M225"/>
@@ -6731,19 +6740,19 @@
         <v>141</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>333</v>
+        <v>354</v>
       </c>
       <c r="D226" t="s">
         <v>141</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="G226" t="s">
         <v>141</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>333</v>
+        <v>370</v>
       </c>
       <c r="I226" s="2"/>
       <c r="M226"/>
@@ -6753,19 +6762,19 @@
         <v>185</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>334</v>
+        <v>355</v>
       </c>
       <c r="D227" t="s">
         <v>185</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>341</v>
+        <v>311</v>
       </c>
       <c r="G227" t="s">
         <v>185</v>
       </c>
       <c r="H227" s="3" t="s">
-        <v>347</v>
+        <v>371</v>
       </c>
       <c r="M227"/>
     </row>
@@ -6774,19 +6783,19 @@
         <v>186</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>335</v>
+        <v>356</v>
       </c>
       <c r="D228" t="s">
         <v>186</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>342</v>
+        <v>363</v>
       </c>
       <c r="G228" t="s">
         <v>186</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>348</v>
+        <v>372</v>
       </c>
       <c r="M228"/>
     </row>
@@ -6795,20 +6804,20 @@
         <v>187</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>336</v>
+        <v>357</v>
       </c>
       <c r="D229" t="s">
         <v>187</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>343</v>
+        <v>364</v>
       </c>
       <c r="F229" s="5"/>
       <c r="G229" t="s">
         <v>187</v>
       </c>
       <c r="H229" s="3" t="s">
-        <v>349</v>
+        <v>373</v>
       </c>
       <c r="I229" s="5"/>
       <c r="J229" s="5"/>
@@ -6819,19 +6828,19 @@
         <v>188</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="D230" t="s">
         <v>188</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>344</v>
+        <v>365</v>
       </c>
       <c r="G230" t="s">
         <v>188</v>
       </c>
       <c r="H230" s="3" t="s">
-        <v>350</v>
+        <v>374</v>
       </c>
       <c r="M230"/>
     </row>

</xml_diff>